<commit_message>
make sfmb and ax not the same
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE21C1C-CBD1-4025-90EB-95596541D549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCB4158-E42A-4514-A9A4-848DC3D26B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1174,7 +1174,7 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,10 +1772,10 @@
         <v>-1</v>
       </c>
       <c r="N9">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="O9">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1787,14 +1787,14 @@
         <v>0.06</v>
       </c>
       <c r="S9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="T9">
         <v>700</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>12.3</v>
+        <v>12.149999999999999</v>
       </c>
       <c r="W9">
         <v>3.9</v>
@@ -3395,10 +3395,10 @@
         <v>-1</v>
       </c>
       <c r="N30">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="O30">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="P30">
         <v>0</v>
@@ -3410,14 +3410,14 @@
         <v>0.06</v>
       </c>
       <c r="S30">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="T30">
         <v>400</v>
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>12.149999999999999</v>
+        <v>12.1</v>
       </c>
       <c r="W30">
         <v>4.4000000000000004</v>

</xml_diff>

<commit_message>
buff suppressors and add jcomp/oppressor
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCB4158-E42A-4514-A9A4-848DC3D26B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C29897-E515-4FA1-8F90-B4BC021DF71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>OLD</t>
   </si>
@@ -330,6 +330,18 @@
   </si>
   <si>
     <t>converted price</t>
+  </si>
+  <si>
+    <t>strike_industries_jcomp_gen2_5.56x45_muzzle_brake</t>
+  </si>
+  <si>
+    <t>strike_industries_oppressor_blast_shield</t>
+  </si>
+  <si>
+    <t>Strike Industries JCOMP Gen2 5.56x45 Muzzle Brake</t>
+  </si>
+  <si>
+    <t>Strike Industries Oppressor Blast Shield</t>
   </si>
 </sst>
 </file>
@@ -472,7 +484,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,6 +664,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -813,9 +837,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1171,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z40"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1355,7 @@
         <v>500</v>
       </c>
       <c r="U3" s="1">
-        <f>M3-R3*20-N3*0.8-O3*0.6-S3*5+Q3*5+P3/300</f>
+        <f>M3-R3*20-N3*0.8-O3*0.6-S3*5+Q3*10+P3/300</f>
         <v>11.75</v>
       </c>
       <c r="W3">
@@ -1375,7 +1405,7 @@
         <v>400</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K40" si="0">C4-H4*20-D4*0.8-E4*0.6-I4*5+G4*5+F4/300</f>
+        <f t="shared" ref="K4:K35" si="0">C4-H4*20-D4*0.8-E4*0.6-I4*5+G4*5+F4/300</f>
         <v>-0.48333333333333323</v>
       </c>
       <c r="M4">
@@ -1403,254 +1433,254 @@
         <v>400</v>
       </c>
       <c r="U4" s="1">
-        <f t="shared" ref="U4:U40" si="1">M4-R4*20-N4*0.8-O4*0.6-S4*5+Q4*5+P4/300</f>
+        <f t="shared" ref="U4:U43" si="1">M4-R4*20-N4*0.8-O4*0.6-S4*5+Q4*10+P4/300</f>
         <v>11.3</v>
       </c>
       <c r="W4">
         <v>3.8</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X40" si="2">W4*0.015</f>
+        <f t="shared" ref="X4:X38" si="2">W4*0.015</f>
         <v>5.6999999999999995E-2</v>
       </c>
       <c r="Y4">
         <v>137</v>
       </c>
       <c r="Z4">
-        <f t="shared" ref="Z4:Z40" si="3">Y4+400</f>
+        <f t="shared" ref="Z4:Z37" si="3">Y4+400</f>
         <v>537</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>-5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>-5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>-5</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>90</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.05</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>0.19</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>-0.1</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>900</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
         <f t="shared" si="0"/>
         <v>-0.75000000000000067</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>-1</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <v>-11</v>
       </c>
-      <c r="O5">
-        <v>-8</v>
-      </c>
-      <c r="P5">
+      <c r="O5" s="2">
+        <v>-10</v>
+      </c>
+      <c r="P5" s="2">
         <v>50</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="2">
         <v>0.04</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="2">
         <v>0.09</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
+      <c r="S5" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="T5" s="2">
         <v>1200</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" si="1"/>
-        <v>11.166666666666666</v>
-      </c>
-      <c r="W5">
+        <v>12.816666666666666</v>
+      </c>
+      <c r="W5" s="2">
         <v>6</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="2">
         <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="2">
         <v>945</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="2">
         <f t="shared" si="3"/>
         <v>1345</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>-6</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>-5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>-8</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>120</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>0.23</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>-0.3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <v>1200</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="3">
         <f t="shared" si="0"/>
         <v>0.59999999999999842</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="2">
         <v>-3</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>-13</v>
       </c>
-      <c r="O6">
-        <v>-9</v>
-      </c>
-      <c r="P6">
+      <c r="O6" s="2">
+        <v>-11</v>
+      </c>
+      <c r="P6" s="2">
         <v>70</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="2">
         <v>0.06</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="2">
         <v>0.12</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="2">
         <v>-0.1</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="2">
         <v>1300</v>
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>11.433333333333332</v>
-      </c>
-      <c r="W6">
+        <v>12.933333333333332</v>
+      </c>
+      <c r="W6" s="2">
         <v>8</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="2">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="2">
         <v>1055</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="2">
         <f t="shared" si="3"/>
         <v>1455</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>-7</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>-5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>-9</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>150</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.15</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>0.27</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
         <v>1500</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
         <v>-1.7500000000000009</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="2">
         <v>-5</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <v>-14</v>
       </c>
-      <c r="O7">
-        <v>-10</v>
-      </c>
-      <c r="P7">
+      <c r="O7" s="2">
+        <v>-12</v>
+      </c>
+      <c r="P7" s="2">
         <v>90</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="2">
         <v>0.1</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="2">
         <v>0.15</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="2">
         <v>-0.2</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="2">
         <v>1400</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>11.000000000000002</v>
-      </c>
-      <c r="W7">
+        <v>12.700000000000001</v>
+      </c>
+      <c r="W7" s="2">
         <v>10</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="2">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="2">
         <v>1165</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="2">
         <f t="shared" si="3"/>
         <v>1565</v>
       </c>
@@ -1733,236 +1763,236 @@
         <v>569</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>-1</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>-3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>-2</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
         <v>0.05</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="6">
         <v>0.05</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <v>800</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="7">
         <f t="shared" si="0"/>
         <v>1.3500000000000003</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="6">
         <v>-1</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="6">
         <v>-13</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="6">
         <v>-7</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
+      <c r="P9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0</v>
+      </c>
+      <c r="R9" s="6">
         <v>0.06</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="6">
         <v>0.05</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="6">
         <v>700</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
         <v>12.149999999999999</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="6">
         <v>3.9</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="6">
         <f t="shared" si="2"/>
         <v>5.8499999999999996E-2</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="6">
         <v>169</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="6">
         <f t="shared" si="3"/>
         <v>569</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>-3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>-5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>-4</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>25</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>0.05</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>0.2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <v>-0.1</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>1200</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="5">
         <f t="shared" si="0"/>
         <v>0.23333333333333323</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>-9</v>
-      </c>
-      <c r="O10">
-        <v>-9</v>
-      </c>
-      <c r="P10">
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>-11</v>
+      </c>
+      <c r="O10" s="4">
+        <v>-10</v>
+      </c>
+      <c r="P10" s="4">
         <v>40</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="4">
         <v>0.02</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="4">
         <v>0.12</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="4">
         <v>-0.05</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="4">
         <v>1000</v>
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>11.683333333333332</v>
-      </c>
-      <c r="W10">
+        <v>12.983333333333333</v>
+      </c>
+      <c r="W10" s="4">
         <v>7.8</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="4">
         <f t="shared" si="2"/>
         <v>0.11699999999999999</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="4">
         <v>250</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="4">
         <f t="shared" si="3"/>
         <v>650</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>-10</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>-4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>-8</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>120</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.15</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>0.23</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>-0.1</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>1500</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="3">
         <f t="shared" si="0"/>
         <v>-4.950000000000002</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="2">
         <v>-4</v>
       </c>
-      <c r="N11">
-        <v>-13</v>
-      </c>
-      <c r="O11">
-        <v>-13</v>
-      </c>
-      <c r="P11">
+      <c r="N11" s="2">
+        <v>-15</v>
+      </c>
+      <c r="O11" s="2">
+        <v>-14</v>
+      </c>
+      <c r="P11" s="2">
         <v>80</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
         <v>0.12</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="2">
         <v>0.25</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="2">
         <v>-0.1</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="2">
         <v>1500</v>
       </c>
       <c r="U11" s="1">
         <f t="shared" si="1"/>
-        <v>10.566666666666666</v>
-      </c>
-      <c r="W11">
+        <v>13.366666666666667</v>
+      </c>
+      <c r="W11" s="2">
         <v>17</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="2">
         <f t="shared" si="2"/>
         <v>0.255</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="2">
         <v>1199</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="2">
         <f t="shared" si="3"/>
         <v>1599</v>
       </c>
@@ -2028,7 +2058,7 @@
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>9.6499999999999986</v>
+        <v>9.85</v>
       </c>
       <c r="W12">
         <v>4.5999999999999996</v>
@@ -2045,80 +2075,80 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>-10</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>-6</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>-7</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>75</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
         <v>0.3</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>-0.7</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <v>1000</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="3">
         <f t="shared" si="0"/>
         <v>-3.2499999999999991</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="2">
         <v>-6</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="2">
         <v>-11</v>
       </c>
-      <c r="O13">
-        <v>-18</v>
-      </c>
-      <c r="P13">
+      <c r="O13" s="2">
+        <v>-19</v>
+      </c>
+      <c r="P13" s="2">
         <v>100</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="2">
         <v>0.3</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="2">
         <v>-0.25</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="2">
         <v>1200</v>
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>9.8833333333333329</v>
-      </c>
-      <c r="W13">
+        <v>11.183333333333335</v>
+      </c>
+      <c r="W13" s="2">
         <v>22</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="2">
         <f t="shared" si="2"/>
         <v>0.32999999999999996</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="2">
         <v>999</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="2">
         <f t="shared" si="3"/>
         <v>1399</v>
       </c>
@@ -2279,80 +2309,80 @@
         <v>514.35</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>-6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>-4</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>-8</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>150</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.01</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>0.25</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <v>-0.5</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
         <v>2000</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="3">
         <f t="shared" si="0"/>
         <v>4.9999999999999989E-2</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="2">
         <v>-5</v>
       </c>
-      <c r="N16">
-        <v>-12</v>
-      </c>
-      <c r="O16">
+      <c r="N16" s="2">
+        <v>-13</v>
+      </c>
+      <c r="O16" s="2">
         <v>-18</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="2">
         <v>90</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="2">
         <v>0.12</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="2">
         <v>0.3</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="2">
         <v>-0.2</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="2">
         <v>1900</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>11.3</v>
-      </c>
-      <c r="W16">
+        <v>12.7</v>
+      </c>
+      <c r="W16" s="2">
         <v>22</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="2">
         <f t="shared" si="2"/>
         <v>0.32999999999999996</v>
       </c>
-      <c r="Y16">
+      <c r="Y16" s="2">
         <v>1685</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="2">
         <f t="shared" si="3"/>
         <v>2085</v>
       </c>
@@ -2435,1146 +2465,1056 @@
         <v>523.75</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>-6</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>-4</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>-4</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>60</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>0.19</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>-0.05</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
         <v>1500</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="3">
         <f t="shared" si="0"/>
         <v>-3.4000000000000008</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="2">
         <v>-2</v>
       </c>
-      <c r="N18">
-        <v>-11</v>
-      </c>
-      <c r="O18">
+      <c r="N18" s="2">
         <v>-12</v>
       </c>
-      <c r="P18">
+      <c r="O18" s="2">
+        <v>-13</v>
+      </c>
+      <c r="P18" s="2">
         <v>60</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="2">
         <v>0.08</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="2">
         <v>0.2</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="2">
         <v>-0.1</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="2">
         <v>1800</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>11.1</v>
-      </c>
-      <c r="W18">
+        <v>12.900000000000002</v>
+      </c>
+      <c r="W18" s="2">
         <v>13.9</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="2">
         <f t="shared" si="2"/>
         <v>0.20849999999999999</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="2">
         <v>1650</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="2">
         <f t="shared" si="3"/>
         <v>2050</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>-10</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>-6</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>-6</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>120</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>0.15</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>0.23</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>-0.1</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="2">
         <v>2500</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="3">
         <f t="shared" si="0"/>
         <v>-4.5500000000000007</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="2">
         <v>-5</v>
       </c>
-      <c r="N19">
-        <v>-14</v>
-      </c>
-      <c r="O19">
+      <c r="N19" s="2">
         <v>-15</v>
       </c>
-      <c r="P19">
+      <c r="O19" s="2">
+        <v>-16</v>
+      </c>
+      <c r="P19" s="2">
         <v>90</v>
       </c>
-      <c r="Q19">
-        <v>0.12</v>
-      </c>
-      <c r="R19">
+      <c r="Q19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="R19" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="2">
         <v>-0.15</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="2">
         <v>2000</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>11.25</v>
-      </c>
-      <c r="W19">
+        <v>13.049999999999999</v>
+      </c>
+      <c r="W19" s="2">
         <v>19.2</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="2">
         <f t="shared" si="2"/>
         <v>0.28799999999999998</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="2">
         <v>1800</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="2">
         <f t="shared" si="3"/>
         <v>2200</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="1">
+        <f>C20-H20*20-D20*0.8-E20*0.6-I20*5+G20*5+F20/300</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>0.03</v>
+      </c>
+      <c r="T20">
+        <v>500</v>
+      </c>
+      <c r="U20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="X20">
+        <f>W20*0.015</f>
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <f>Y20+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1">
+        <f>C21-H21*20-D21*0.8-E21*0.6-I21*5+G21*5+F21/300</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0.04</v>
+      </c>
+      <c r="T21">
+        <v>500</v>
+      </c>
+      <c r="U21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="X21">
+        <f>W21*0.015</f>
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <f>Y21+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>56</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>-2</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>-4</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>-3</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>100</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>0.1</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>400</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K22" s="1">
         <f t="shared" si="0"/>
         <v>1.6833333333333333</v>
       </c>
-      <c r="M20">
+      <c r="M22">
         <v>1</v>
       </c>
-      <c r="N20">
+      <c r="N22">
         <v>-4</v>
       </c>
-      <c r="O20">
+      <c r="O22">
         <v>-14</v>
       </c>
-      <c r="P20">
+      <c r="P22">
         <v>40</v>
       </c>
-      <c r="Q20">
+      <c r="Q22">
         <v>0.06</v>
       </c>
-      <c r="R20">
+      <c r="R22">
         <v>0.1</v>
       </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
         <v>300</v>
       </c>
-      <c r="U20" s="1">
+      <c r="U22" s="1">
         <f t="shared" si="1"/>
-        <v>11.033333333333335</v>
-      </c>
-      <c r="W20">
+        <v>11.333333333333334</v>
+      </c>
+      <c r="W22">
         <v>7.2</v>
       </c>
-      <c r="X20">
+      <c r="X22">
         <f t="shared" si="2"/>
         <v>0.108</v>
       </c>
-      <c r="Y20">
+      <c r="Y22">
         <v>25.95</v>
       </c>
-      <c r="Z20">
+      <c r="Z22">
         <f t="shared" si="3"/>
         <v>425.95</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>58</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>-2</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>-4</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <v>-4</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>100</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>0.05</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
         <f t="shared" si="0"/>
         <v>2.2833333333333332</v>
       </c>
-      <c r="M21">
+      <c r="M23">
         <v>2</v>
       </c>
-      <c r="N21">
-        <v>-6</v>
-      </c>
-      <c r="O21">
-        <v>-7</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
+      <c r="N23">
+        <v>-5</v>
+      </c>
+      <c r="O23">
+        <v>-5</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
         <v>0.03</v>
       </c>
-      <c r="S21">
+      <c r="S23">
         <v>0.1</v>
       </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21" s="1">
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>9.9000000000000021</v>
-      </c>
-      <c r="W21">
+        <v>7.9</v>
+      </c>
+      <c r="W23">
         <v>1.9</v>
       </c>
-      <c r="X21">
+      <c r="X23">
         <f t="shared" si="2"/>
         <v>2.8499999999999998E-2</v>
       </c>
-      <c r="Y21">
+      <c r="Y23">
         <v>8.99</v>
       </c>
-      <c r="Z21">
+      <c r="Z23">
         <f t="shared" si="3"/>
         <v>408.99</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C22">
+      <c r="C24" s="2">
         <v>-7</v>
       </c>
-      <c r="D22">
+      <c r="D24" s="2">
         <v>-6</v>
       </c>
-      <c r="E22">
+      <c r="E24" s="2">
         <v>-7</v>
       </c>
-      <c r="F22">
+      <c r="F24" s="2">
         <v>140</v>
       </c>
-      <c r="G22">
+      <c r="G24" s="2">
         <v>0.15</v>
       </c>
-      <c r="H22">
+      <c r="H24" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I22">
+      <c r="I24" s="2">
         <v>-0.3</v>
       </c>
-      <c r="J22">
+      <c r="J24" s="2">
         <v>2000</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K24" s="3">
         <f t="shared" si="0"/>
         <v>-0.88333333333333386</v>
       </c>
-      <c r="M22">
+      <c r="M24" s="2">
         <v>-5</v>
       </c>
-      <c r="N22">
-        <v>-11</v>
-      </c>
-      <c r="O22">
-        <v>-15</v>
-      </c>
-      <c r="P22">
+      <c r="N24" s="2">
+        <v>-12</v>
+      </c>
+      <c r="O24" s="2">
+        <v>-14</v>
+      </c>
+      <c r="P24" s="2">
         <v>100</v>
       </c>
-      <c r="Q22">
+      <c r="Q24" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="R22">
+      <c r="R24" s="2">
         <v>0.19</v>
       </c>
-      <c r="S22">
+      <c r="S24" s="2">
         <v>-0.2</v>
       </c>
-      <c r="T22">
+      <c r="T24" s="2">
         <v>1300</v>
       </c>
-      <c r="U22" s="1">
+      <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>11.033333333333333</v>
-      </c>
-      <c r="W22">
+        <v>11.933333333333335</v>
+      </c>
+      <c r="W24" s="2">
         <v>12.8</v>
       </c>
-      <c r="X22">
+      <c r="X24" s="2">
         <f t="shared" si="2"/>
         <v>0.192</v>
       </c>
-      <c r="Y22">
+      <c r="Y24" s="2">
         <v>999</v>
       </c>
-      <c r="Z22">
+      <c r="Z24" s="2">
         <f t="shared" si="3"/>
         <v>1399</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>-2</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>-2</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>-2</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>80</v>
       </c>
-      <c r="G23">
+      <c r="G25">
         <v>0.05</v>
       </c>
-      <c r="H23">
+      <c r="H25">
         <v>0.12</v>
       </c>
-      <c r="I23">
+      <c r="I25">
         <v>0.15</v>
       </c>
-      <c r="J23">
+      <c r="J25">
         <v>1000</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K25" s="1">
         <f t="shared" si="0"/>
         <v>-1.8333333333333339</v>
       </c>
-      <c r="M23">
+      <c r="M25">
         <v>-2</v>
       </c>
-      <c r="N23">
+      <c r="N25">
         <v>-2</v>
       </c>
-      <c r="O23">
+      <c r="O25">
         <v>-2</v>
       </c>
-      <c r="P23">
+      <c r="P25">
         <v>80</v>
       </c>
-      <c r="Q23">
+      <c r="Q25">
         <v>0.08</v>
       </c>
-      <c r="R23">
+      <c r="R25">
         <v>0.16</v>
       </c>
-      <c r="S23">
+      <c r="S25">
         <v>0.24</v>
       </c>
-      <c r="T23">
+      <c r="T25">
         <v>600</v>
       </c>
-      <c r="U23" s="1">
+      <c r="U25" s="1">
         <f t="shared" si="1"/>
-        <v>-2.933333333333334</v>
-      </c>
-      <c r="X23">
+        <v>-2.5333333333333341</v>
+      </c>
+      <c r="X25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y23">
+      <c r="Y25">
         <v>59.99</v>
       </c>
-      <c r="Z23">
+      <c r="Z25">
         <f t="shared" si="3"/>
         <v>459.99</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="C24">
+      <c r="C26">
         <v>-1.5</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>-1</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <v>-1</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <v>60</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>0.09</v>
       </c>
-      <c r="I24">
+      <c r="I26">
         <v>0.1</v>
       </c>
-      <c r="J24">
+      <c r="J26">
         <v>750</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K26" s="1">
         <f t="shared" si="0"/>
         <v>-2.1999999999999997</v>
       </c>
-      <c r="M24">
+      <c r="M26">
         <v>-1</v>
       </c>
-      <c r="N24">
+      <c r="N26">
         <v>-1</v>
       </c>
-      <c r="O24">
+      <c r="O26">
         <v>-1</v>
       </c>
-      <c r="P24">
+      <c r="P26">
         <v>40</v>
       </c>
-      <c r="Q24">
+      <c r="Q26">
         <v>0.04</v>
       </c>
-      <c r="R24">
+      <c r="R26">
         <v>0.08</v>
       </c>
-      <c r="S24">
+      <c r="S26">
         <v>0.12</v>
       </c>
-      <c r="T24">
+      <c r="T26">
         <v>500</v>
       </c>
-      <c r="U24" s="1">
+      <c r="U26" s="1">
         <f t="shared" si="1"/>
-        <v>-1.466666666666667</v>
-      </c>
-      <c r="X24">
+        <v>-1.2666666666666671</v>
+      </c>
+      <c r="X26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y24">
+      <c r="Y26">
         <v>44.99</v>
       </c>
-      <c r="Z24">
+      <c r="Z26">
         <f t="shared" si="3"/>
         <v>444.99</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>66</v>
       </c>
-      <c r="C25">
+      <c r="C27">
         <v>-1</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <v>40</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>0.06</v>
       </c>
-      <c r="I25">
+      <c r="I27">
         <v>0.05</v>
       </c>
-      <c r="J25">
+      <c r="J27">
         <v>500</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K27" s="1">
         <f t="shared" si="0"/>
         <v>-2.3166666666666669</v>
       </c>
-      <c r="M25">
+      <c r="M27">
         <v>-0.5</v>
       </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
         <v>20</v>
       </c>
-      <c r="Q25">
+      <c r="Q27">
         <v>0.02</v>
       </c>
-      <c r="R25">
+      <c r="R27">
         <v>0.04</v>
       </c>
-      <c r="S25">
+      <c r="S27">
         <v>0.06</v>
       </c>
-      <c r="T25">
+      <c r="T27">
         <v>400</v>
       </c>
-      <c r="U25" s="1">
+      <c r="U27" s="1">
         <f t="shared" si="1"/>
-        <v>-1.4333333333333333</v>
-      </c>
-      <c r="X25">
+        <v>-1.3333333333333335</v>
+      </c>
+      <c r="X27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y25">
+      <c r="Y27">
         <v>29.99</v>
       </c>
-      <c r="Z25">
+      <c r="Z27">
         <f t="shared" si="3"/>
         <v>429.99</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>67</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <v>-1</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
         <v>2</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>5</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
         <v>0.03</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>0.1</v>
       </c>
-      <c r="J26">
+      <c r="J28">
         <v>300</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K28" s="1">
         <f t="shared" si="0"/>
         <v>-3.2833333333333332</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>-3</v>
+      </c>
+      <c r="O28">
         <v>-4</v>
       </c>
-      <c r="O26">
-        <v>-5</v>
-      </c>
-      <c r="P26">
+      <c r="P28">
         <v>20</v>
       </c>
-      <c r="Q26">
+      <c r="Q28">
         <v>0.02</v>
       </c>
-      <c r="R26">
+      <c r="R28">
         <v>0.03</v>
       </c>
-      <c r="S26">
+      <c r="S28">
         <v>0.05</v>
       </c>
-      <c r="T26">
+      <c r="T28">
         <v>300</v>
       </c>
-      <c r="U26" s="1">
+      <c r="U28" s="1">
         <f t="shared" si="1"/>
-        <v>5.5166666666666657</v>
-      </c>
-      <c r="X26">
+        <v>4.2166666666666668</v>
+      </c>
+      <c r="X28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z26">
+      <c r="Z28">
         <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C27">
+      <c r="C29" s="2">
         <v>-16</v>
       </c>
-      <c r="D27">
+      <c r="D29" s="2">
         <v>-6</v>
       </c>
-      <c r="E27">
+      <c r="E29" s="2">
         <v>-12</v>
       </c>
-      <c r="F27">
+      <c r="F29" s="2">
         <v>200</v>
       </c>
-      <c r="G27">
+      <c r="G29" s="2">
         <v>0.1</v>
       </c>
-      <c r="H27">
+      <c r="H29" s="2">
         <v>0.3</v>
       </c>
-      <c r="I27">
+      <c r="I29" s="2">
         <v>-0.3</v>
       </c>
-      <c r="J27">
+      <c r="J29" s="2">
         <v>1500</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K29" s="3">
         <f t="shared" si="0"/>
         <v>-7.333333333333333</v>
       </c>
-      <c r="M27">
+      <c r="M29" s="2">
         <v>-5</v>
       </c>
-      <c r="N27">
-        <v>-13</v>
-      </c>
-      <c r="O27">
-        <v>-15</v>
-      </c>
-      <c r="P27">
+      <c r="N29" s="2">
+        <v>-16</v>
+      </c>
+      <c r="O29" s="2">
+        <v>-11</v>
+      </c>
+      <c r="P29" s="2">
         <v>90</v>
       </c>
-      <c r="Q27">
-        <v>0.1</v>
-      </c>
-      <c r="R27">
+      <c r="Q29" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="R29" s="2">
         <v>0.24</v>
       </c>
-      <c r="S27">
+      <c r="S29" s="2">
         <v>-0.15</v>
       </c>
-      <c r="T27">
+      <c r="T29" s="2">
         <v>1400</v>
       </c>
-      <c r="U27" s="1">
+      <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>11.15</v>
-      </c>
-      <c r="W27">
+        <v>11.85</v>
+      </c>
+      <c r="W29" s="2">
         <v>17.399999999999999</v>
       </c>
-      <c r="X27">
+      <c r="X29" s="2">
         <f t="shared" si="2"/>
         <v>0.26099999999999995</v>
       </c>
-      <c r="Y27">
+      <c r="Y29" s="2">
         <v>1099</v>
       </c>
-      <c r="Z27">
+      <c r="Z29" s="2">
         <f t="shared" si="3"/>
         <v>1499</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>71</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>72</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>-1</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>-3</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>-1</v>
       </c>
-      <c r="F28">
+      <c r="F30">
         <v>5</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>0.04</v>
       </c>
-      <c r="I28">
+      <c r="I30">
         <v>0.1</v>
       </c>
-      <c r="J28">
+      <c r="J30">
         <v>300</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K30" s="1">
         <f t="shared" si="0"/>
         <v>0.7166666666666669</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
         <v>-12</v>
       </c>
-      <c r="O28">
+      <c r="O30">
         <v>-6</v>
       </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
         <v>0.05</v>
       </c>
-      <c r="S28">
+      <c r="S30">
         <v>0.1</v>
       </c>
-      <c r="T28">
+      <c r="T30">
         <v>500</v>
       </c>
-      <c r="U28" s="1">
+      <c r="U30" s="1">
         <f t="shared" si="1"/>
         <v>11.700000000000001</v>
       </c>
-      <c r="W28">
+      <c r="W30">
         <v>3.84</v>
       </c>
-      <c r="X28">
+      <c r="X30">
         <f t="shared" si="2"/>
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="Y28">
+      <c r="Y30">
         <v>151</v>
       </c>
-      <c r="Z28">
+      <c r="Z30">
         <f t="shared" si="3"/>
         <v>551</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C29">
+      <c r="C31" s="2">
         <v>-11</v>
       </c>
-      <c r="D29">
+      <c r="D31" s="2">
         <v>-3</v>
       </c>
-      <c r="E29">
+      <c r="E31" s="2">
         <v>-9</v>
       </c>
-      <c r="F29">
+      <c r="F31" s="2">
         <v>100</v>
       </c>
-      <c r="G29">
+      <c r="G31" s="2">
         <v>0.2</v>
       </c>
-      <c r="H29">
+      <c r="H31" s="2">
         <v>0.24</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
         <v>1300</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K31" s="3">
         <f t="shared" si="0"/>
         <v>-6.666666666666667</v>
       </c>
-      <c r="M29">
+      <c r="M31" s="2">
         <v>-6</v>
       </c>
-      <c r="N29">
+      <c r="N31" s="2">
         <v>-15</v>
       </c>
-      <c r="O29">
-        <v>-14</v>
-      </c>
-      <c r="P29">
+      <c r="O31" s="2">
+        <v>-15</v>
+      </c>
+      <c r="P31" s="2">
         <v>90</v>
       </c>
-      <c r="Q29">
+      <c r="Q31" s="2">
         <v>0.16</v>
       </c>
-      <c r="R29">
+      <c r="R31" s="2">
         <v>0.25</v>
       </c>
-      <c r="S29">
+      <c r="S31" s="2">
         <v>-0.1</v>
       </c>
-      <c r="T29">
+      <c r="T31" s="2">
         <v>1200</v>
       </c>
-      <c r="U29" s="1">
+      <c r="U31" s="1">
         <f t="shared" si="1"/>
-        <v>11.000000000000002</v>
-      </c>
-      <c r="W29">
+        <v>12.4</v>
+      </c>
+      <c r="W31" s="2">
         <v>16.760000000000002</v>
       </c>
-      <c r="X29">
+      <c r="X31" s="2">
         <f t="shared" si="2"/>
         <v>0.25140000000000001</v>
       </c>
-      <c r="Y29">
+      <c r="Y31" s="2">
         <v>899.99</v>
       </c>
-      <c r="Z29">
+      <c r="Z31" s="2">
         <f t="shared" si="3"/>
         <v>1299.99</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>76</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>-2</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>-5</v>
       </c>
-      <c r="E30">
+      <c r="E32">
         <v>-6</v>
       </c>
-      <c r="F30">
+      <c r="F32">
         <v>50</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>0.05</v>
       </c>
-      <c r="I30">
+      <c r="I32">
         <v>0.2</v>
       </c>
-      <c r="J30">
+      <c r="J32">
         <v>750</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K32" s="1">
         <f t="shared" si="0"/>
         <v>3.7666666666666662</v>
       </c>
-      <c r="M30">
+      <c r="M32">
         <v>-1</v>
       </c>
-      <c r="N30">
+      <c r="N32">
         <v>-14</v>
       </c>
-      <c r="O30">
+      <c r="O32">
         <v>-6</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
         <v>0.06</v>
       </c>
-      <c r="S30">
+      <c r="S32">
         <v>0.1</v>
       </c>
-      <c r="T30">
+      <c r="T32">
         <v>400</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U32" s="1">
         <f t="shared" si="1"/>
         <v>12.1</v>
       </c>
-      <c r="W30">
+      <c r="W32">
         <v>4.4000000000000004</v>
       </c>
-      <c r="X30">
+      <c r="X32">
         <f t="shared" si="2"/>
         <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="Z30">
-        <f t="shared" si="3"/>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31">
-        <v>-0.5</v>
-      </c>
-      <c r="D31">
-        <v>-5</v>
-      </c>
-      <c r="E31">
-        <v>-5</v>
-      </c>
-      <c r="F31">
-        <v>30</v>
-      </c>
-      <c r="G31">
-        <v>0.05</v>
-      </c>
-      <c r="H31">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I31">
-        <v>0.05</v>
-      </c>
-      <c r="J31">
-        <v>1000</v>
-      </c>
-      <c r="K31" s="1">
-        <f t="shared" si="0"/>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
-      </c>
-      <c r="N31">
-        <v>-7</v>
-      </c>
-      <c r="O31">
-        <v>-12</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S31">
-        <v>0.05</v>
-      </c>
-      <c r="T31">
-        <v>500</v>
-      </c>
-      <c r="U31" s="1">
-        <f t="shared" si="1"/>
-        <v>12.149999999999999</v>
-      </c>
-      <c r="W31">
-        <v>4.8</v>
-      </c>
-      <c r="X31">
-        <f t="shared" si="2"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="Y31">
-        <v>64.989999999999995</v>
-      </c>
-      <c r="Z31">
-        <f t="shared" si="3"/>
-        <v>464.99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32">
-        <v>-6.5</v>
-      </c>
-      <c r="D32">
-        <v>-6</v>
-      </c>
-      <c r="E32">
-        <v>-10</v>
-      </c>
-      <c r="F32">
-        <v>250</v>
-      </c>
-      <c r="G32">
-        <v>0.1</v>
-      </c>
-      <c r="H32">
-        <v>0.27</v>
-      </c>
-      <c r="I32">
-        <v>-0.5</v>
-      </c>
-      <c r="J32">
-        <v>2000</v>
-      </c>
-      <c r="K32" s="1">
-        <f t="shared" si="0"/>
-        <v>2.7333333333333338</v>
-      </c>
-      <c r="M32">
-        <v>-2</v>
-      </c>
-      <c r="N32">
-        <v>-10</v>
-      </c>
-      <c r="O32">
-        <v>-15</v>
-      </c>
-      <c r="P32">
-        <v>60</v>
-      </c>
-      <c r="Q32">
-        <v>0.08</v>
-      </c>
-      <c r="R32">
-        <v>0.27</v>
-      </c>
-      <c r="S32">
-        <v>-0.05</v>
-      </c>
-      <c r="T32">
-        <v>1500</v>
-      </c>
-      <c r="U32" s="1">
-        <f t="shared" si="1"/>
-        <v>10.45</v>
-      </c>
-      <c r="X32">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
       <c r="Z32">
         <f t="shared" si="3"/>
@@ -3583,263 +3523,248 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C33">
-        <v>-8</v>
+        <v>-0.5</v>
       </c>
       <c r="D33">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="E33">
-        <v>-12</v>
+        <v>-5</v>
       </c>
       <c r="F33">
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="G33">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="H33">
-        <v>0.32</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I33">
-        <v>-0.5</v>
+        <v>0.05</v>
       </c>
       <c r="J33">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="0"/>
-        <v>2.4333333333333327</v>
+        <v>5.1999999999999993</v>
       </c>
       <c r="M33">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="N33">
+        <v>-7</v>
+      </c>
+      <c r="O33">
         <v>-12</v>
       </c>
-      <c r="O33">
-        <v>-16</v>
-      </c>
       <c r="P33">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q33">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="R33">
-        <v>0.32</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="S33">
-        <v>-0.1</v>
+        <v>0.05</v>
       </c>
       <c r="T33">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="U33" s="1">
         <f t="shared" si="1"/>
-        <v>10.166666666666668</v>
+        <v>12.149999999999999</v>
       </c>
       <c r="W33">
-        <v>22.2</v>
+        <v>4.8</v>
       </c>
       <c r="X33">
         <f t="shared" si="2"/>
-        <v>0.33299999999999996</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="Y33">
-        <v>797.99</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="Z33">
         <f t="shared" si="3"/>
-        <v>1197.99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34">
+        <v>464.99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="2">
+        <v>-6.5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>-6</v>
+      </c>
+      <c r="E34" s="2">
+        <v>-10</v>
+      </c>
+      <c r="F34" s="2">
+        <v>250</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="I34" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="J34" s="2">
+        <v>2000</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7333333333333338</v>
+      </c>
+      <c r="M34" s="2">
         <v>-2</v>
       </c>
-      <c r="D34">
-        <v>-6</v>
-      </c>
-      <c r="E34">
-        <v>-5</v>
-      </c>
-      <c r="F34">
+      <c r="N34" s="2">
+        <v>-10</v>
+      </c>
+      <c r="O34" s="2">
+        <v>-16</v>
+      </c>
+      <c r="P34" s="2">
         <v>50</v>
       </c>
-      <c r="G34">
-        <v>0.05</v>
-      </c>
-      <c r="H34">
-        <v>0.05</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="K34" s="1">
-        <f t="shared" si="0"/>
-        <v>5.2166666666666677</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34">
-        <v>-9</v>
-      </c>
-      <c r="O34">
-        <v>-7</v>
-      </c>
-      <c r="P34">
-        <v>50</v>
-      </c>
-      <c r="Q34">
-        <v>0.02</v>
-      </c>
-      <c r="R34">
-        <v>0.05</v>
-      </c>
-      <c r="S34">
-        <v>0</v>
+      <c r="Q34" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="R34" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="S34" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="T34" s="2">
+        <v>1500</v>
       </c>
       <c r="U34" s="1">
         <f t="shared" si="1"/>
-        <v>11.666666666666666</v>
-      </c>
-      <c r="X34">
+        <v>11.416666666666666</v>
+      </c>
+      <c r="X34" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z34">
+      <c r="Z34" s="2">
         <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35">
-        <v>-2</v>
-      </c>
-      <c r="D35">
+    <row r="35" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="2">
         <v>-8</v>
       </c>
-      <c r="E35">
-        <v>-3</v>
-      </c>
-      <c r="F35">
-        <v>120</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0.06</v>
-      </c>
-      <c r="I35">
-        <v>0.05</v>
-      </c>
-      <c r="J35">
-        <v>500</v>
-      </c>
-      <c r="K35" s="1">
+      <c r="D35" s="2">
+        <v>-6</v>
+      </c>
+      <c r="E35" s="2">
+        <v>-12</v>
+      </c>
+      <c r="F35" s="2">
+        <v>400</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="I35" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="J35" s="2">
+        <v>2000</v>
+      </c>
+      <c r="K35" s="3">
         <f t="shared" si="0"/>
-        <v>5.15</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35">
-        <v>-8</v>
-      </c>
-      <c r="O35">
-        <v>-9</v>
-      </c>
-      <c r="P35">
-        <v>60</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>0.06</v>
-      </c>
-      <c r="S35">
-        <v>0.05</v>
-      </c>
-      <c r="T35">
-        <v>500</v>
+        <v>2.4333333333333327</v>
+      </c>
+      <c r="M35" s="2">
+        <v>-4</v>
+      </c>
+      <c r="N35" s="2">
+        <v>-12</v>
+      </c>
+      <c r="O35" s="2">
+        <v>-17</v>
+      </c>
+      <c r="P35" s="2">
+        <v>70</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="S35" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="T35" s="2">
+        <v>1600</v>
       </c>
       <c r="U35" s="1">
         <f t="shared" si="1"/>
-        <v>11.549999999999999</v>
-      </c>
-      <c r="X35">
+        <v>11.333333333333332</v>
+      </c>
+      <c r="W35" s="2">
+        <v>22.2</v>
+      </c>
+      <c r="X35" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z35">
+        <v>0.33299999999999996</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>797.99</v>
+      </c>
+      <c r="Z35" s="2">
         <f t="shared" si="3"/>
-        <v>400</v>
+        <v>1197.99</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36">
+        <v>94</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="M36">
         <v>-1</v>
       </c>
-      <c r="D36">
-        <v>-5</v>
-      </c>
-      <c r="E36">
-        <v>-7</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>750</v>
-      </c>
-      <c r="K36" s="1">
-        <f t="shared" si="0"/>
-        <v>5.8</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
       <c r="N36">
+        <v>-12</v>
+      </c>
+      <c r="O36">
         <v>-9</v>
-      </c>
-      <c r="O36">
-        <v>-10</v>
       </c>
       <c r="P36">
         <v>0</v>
@@ -3851,211 +3776,419 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="S36">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="T36">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="U36" s="1">
         <f t="shared" si="1"/>
-        <v>11.8</v>
+        <v>12.100000000000001</v>
+      </c>
+      <c r="W36">
+        <v>3.8</v>
       </c>
       <c r="X36">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6999999999999995E-2</v>
+      </c>
+      <c r="Y36">
+        <v>200</v>
       </c>
       <c r="Z36">
         <f t="shared" si="3"/>
-        <v>400</v>
+        <v>600</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37">
-        <v>-2</v>
-      </c>
-      <c r="D37">
-        <v>5</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="F37">
-        <v>-50</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
+        <v>101</v>
+      </c>
+      <c r="M37">
+        <v>-1</v>
+      </c>
+      <c r="N37">
+        <v>-9</v>
+      </c>
+      <c r="O37">
+        <v>-12</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
         <v>0.05</v>
       </c>
-      <c r="I37">
-        <v>0.1</v>
-      </c>
-      <c r="J37">
-        <v>1500</v>
-      </c>
-      <c r="K37" s="1">
-        <f t="shared" si="0"/>
-        <v>-10.666666666666666</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>30</v>
-      </c>
-      <c r="Q37">
-        <v>0.02</v>
-      </c>
-      <c r="R37">
-        <v>0.04</v>
-      </c>
       <c r="S37">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="T37">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>-1.0999999999999999</v>
+        <v>12.149999999999999</v>
+      </c>
+      <c r="W37">
+        <v>3.6</v>
       </c>
       <c r="X37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Y37">
+        <v>43.95</v>
       </c>
       <c r="Z37">
         <f t="shared" si="3"/>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>91</v>
-      </c>
-      <c r="K38" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="R38">
-        <v>0.03</v>
-      </c>
-      <c r="T38">
-        <v>500</v>
+        <v>443.95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M38" s="4">
+        <v>0</v>
+      </c>
+      <c r="N38" s="4">
+        <v>-9</v>
+      </c>
+      <c r="O38" s="4">
+        <v>-13</v>
+      </c>
+      <c r="P38" s="4">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="R38" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S38" s="4">
+        <v>-0.05</v>
+      </c>
+      <c r="T38" s="4">
+        <v>1000</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="X38">
+        <v>12.716666666666665</v>
+      </c>
+      <c r="W38" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="X38" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z38">
-        <f t="shared" si="3"/>
-        <v>400</v>
+        <v>0.14249999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>92</v>
-      </c>
-      <c r="K39" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="R39">
-        <v>0.04</v>
-      </c>
-      <c r="T39">
-        <v>500</v>
-      </c>
       <c r="U39" s="1">
         <f t="shared" si="1"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="X39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z39">
-        <f>Y39+400</f>
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="C40">
+        <v>-2</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>-50</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0.05</v>
+      </c>
+      <c r="I40">
+        <v>0.1</v>
+      </c>
+      <c r="J40">
+        <v>1500</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C40-H40*20-D40*0.8-E40*0.6-I40*5+G40*5+F40/300</f>
+        <v>-10.666666666666666</v>
       </c>
       <c r="M40">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="O40">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="P40">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q40">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="R40">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="S40">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="T40">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="U40" s="1">
         <f t="shared" si="1"/>
-        <v>12.150000000000002</v>
-      </c>
-      <c r="W40">
-        <v>3.8</v>
+        <v>-1</v>
       </c>
       <c r="X40">
-        <f t="shared" si="2"/>
-        <v>5.6999999999999995E-2</v>
-      </c>
-      <c r="Y40">
-        <v>200</v>
+        <f>W40*0.015</f>
+        <v>0</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
+        <f>Y40+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41">
+        <v>-2</v>
+      </c>
+      <c r="D41">
+        <v>-6</v>
+      </c>
+      <c r="E41">
+        <v>-5</v>
+      </c>
+      <c r="F41">
+        <v>50</v>
+      </c>
+      <c r="G41">
+        <v>0.05</v>
+      </c>
+      <c r="H41">
+        <v>0.05</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
+        <f>C41-H41*20-D41*0.8-E41*0.6-I41*5+G41*5+F41/300</f>
+        <v>5.2166666666666677</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>-9</v>
+      </c>
+      <c r="O41">
+        <v>-7</v>
+      </c>
+      <c r="P41">
+        <v>50</v>
+      </c>
+      <c r="Q41">
+        <v>0.02</v>
+      </c>
+      <c r="R41">
+        <v>0.05</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="U41" s="1">
+        <f t="shared" si="1"/>
+        <v>11.766666666666666</v>
+      </c>
+      <c r="X41">
+        <f>W41*0.015</f>
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <f>Y41+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42">
+        <v>-2</v>
+      </c>
+      <c r="D42">
+        <v>-8</v>
+      </c>
+      <c r="E42">
+        <v>-3</v>
+      </c>
+      <c r="F42">
+        <v>120</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0.06</v>
+      </c>
+      <c r="I42">
+        <v>0.05</v>
+      </c>
+      <c r="J42">
+        <v>500</v>
+      </c>
+      <c r="K42" s="1">
+        <f>C42-H42*20-D42*0.8-E42*0.6-I42*5+G42*5+F42/300</f>
+        <v>5.15</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>-8</v>
+      </c>
+      <c r="O42">
+        <v>-9</v>
+      </c>
+      <c r="P42">
+        <v>60</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0.06</v>
+      </c>
+      <c r="S42">
+        <v>0.05</v>
+      </c>
+      <c r="T42">
+        <v>500</v>
+      </c>
+      <c r="U42" s="1">
+        <f t="shared" si="1"/>
+        <v>11.549999999999999</v>
+      </c>
+      <c r="X42">
+        <f>W42*0.015</f>
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <f>Y42+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43">
+        <v>-1</v>
+      </c>
+      <c r="D43">
+        <v>-5</v>
+      </c>
+      <c r="E43">
+        <v>-7</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>750</v>
+      </c>
+      <c r="K43" s="1">
+        <f>C43-H43*20-D43*0.8-E43*0.6-I43*5+G43*5+F43/300</f>
+        <v>5.8</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>-9</v>
+      </c>
+      <c r="O43">
+        <v>-10</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>750</v>
+      </c>
+      <c r="U43" s="1">
+        <f t="shared" si="1"/>
+        <v>11.8</v>
+      </c>
+      <c r="X43">
+        <f>W43*0.015</f>
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <f>Y43+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U44" s="1"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
go back a bit on the suppressors
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C29897-E515-4FA1-8F90-B4BC021DF71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4450FB6E-EC9F-485A-9028-B33E002217D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
   <si>
     <t>OLD</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>Strike Industries Oppressor Blast Shield</t>
+  </si>
+  <si>
+    <t>steyr_breezer_ums_5.56x45_aug_suppressor</t>
+  </si>
+  <si>
+    <t>Steyr Breezer UMS 5.56x45 AUG Suppressor</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1210,7 @@
   <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,22 +1238,22 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -1259,22 +1265,22 @@
         <v>13</v>
       </c>
       <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
         <v>16</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" t="s">
-        <v>19</v>
       </c>
       <c r="T2" t="s">
         <v>20</v>
@@ -1306,56 +1312,56 @@
         <v>-3</v>
       </c>
       <c r="D3">
+        <v>0.09</v>
+      </c>
+      <c r="E3">
         <v>-7</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3">
+        <v>0.05</v>
+      </c>
+      <c r="I3">
         <v>40</v>
-      </c>
-      <c r="G3">
-        <v>0.05</v>
-      </c>
-      <c r="H3">
-        <v>0.09</v>
-      </c>
-      <c r="I3">
-        <v>0.1</v>
       </c>
       <c r="J3">
         <v>750</v>
       </c>
       <c r="K3" s="1">
-        <f>C3-H3*20-D3*0.8-E3*0.6-I3*5+G3*5+F3/300</f>
+        <f>C3-D3*20-E3*0.8-F3*0.6-G3*5+H3*5+I3/300</f>
         <v>3.0833333333333339</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O3">
         <v>-6</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>-11</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
       <c r="Q3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>500</v>
       </c>
       <c r="U3" s="1">
-        <f>M3-R3*20-N3*0.8-O3*0.6-S3*5+Q3*10+P3/300</f>
+        <f>M3-N3*20-O3*0.8-P3*0.6-Q3*5+R3*10+S3/300</f>
         <v>11.75</v>
       </c>
       <c r="W3">
@@ -1384,70 +1390,70 @@
         <v>-1</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>0.02</v>
       </c>
       <c r="E4">
         <v>-1</v>
       </c>
       <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>0.1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>5</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0.02</v>
-      </c>
-      <c r="I4">
-        <v>0.1</v>
       </c>
       <c r="J4">
         <v>400</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K35" si="0">C4-H4*20-D4*0.8-E4*0.6-I4*5+G4*5+F4/300</f>
+        <f>C4-D4*20-E4*0.8-F4*0.6-G4*5+H4*5+I4/300</f>
         <v>-0.48333333333333323</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
+        <v>0.05</v>
+      </c>
+      <c r="O4">
         <v>-10</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>-8</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
       <c r="Q4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>400</v>
       </c>
       <c r="U4" s="1">
-        <f t="shared" ref="U4:U43" si="1">M4-R4*20-N4*0.8-O4*0.6-S4*5+Q4*10+P4/300</f>
+        <f>M4-N4*20-O4*0.8-P4*0.6-Q4*5+R4*10+S4/300</f>
         <v>11.3</v>
       </c>
       <c r="W4">
         <v>3.8</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X38" si="2">W4*0.015</f>
+        <f t="shared" ref="X4:X38" si="0">W4*0.015</f>
         <v>5.6999999999999995E-2</v>
       </c>
       <c r="Y4">
         <v>137</v>
       </c>
       <c r="Z4">
-        <f t="shared" ref="Z4:Z37" si="3">Y4+400</f>
+        <f t="shared" ref="Z4:Z37" si="1">Y4+400</f>
         <v>537</v>
       </c>
     </row>
@@ -1462,70 +1468,70 @@
         <v>-5</v>
       </c>
       <c r="D5" s="2">
-        <v>-5</v>
+        <v>0.19</v>
       </c>
       <c r="E5" s="2">
         <v>-5</v>
       </c>
       <c r="F5" s="2">
+        <v>-5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="2">
         <v>90</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="I5" s="2">
-        <v>-0.1</v>
       </c>
       <c r="J5" s="2">
         <v>900</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="0"/>
+        <f>C5-D5*20-E5*0.8-F5*0.6-G5*5+H5*5+I5/300</f>
         <v>-0.75000000000000067</v>
       </c>
       <c r="M5" s="2">
         <v>-1</v>
       </c>
       <c r="N5" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="O5" s="2">
         <v>-11</v>
       </c>
-      <c r="O5" s="2">
-        <v>-10</v>
-      </c>
       <c r="P5" s="2">
+        <v>-9</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="S5" s="2">
         <v>50</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="S5" s="2">
-        <v>-0.05</v>
       </c>
       <c r="T5" s="2">
         <v>1200</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" si="1"/>
-        <v>12.816666666666666</v>
+        <f>M5-N5*20-O5*0.8-P5*0.6-Q5*5+R5*10+S5/300</f>
+        <v>12.216666666666667</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
       </c>
       <c r="X5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
       <c r="Y5" s="2">
         <v>945</v>
       </c>
       <c r="Z5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1345</v>
       </c>
     </row>
@@ -1540,70 +1546,70 @@
         <v>-6</v>
       </c>
       <c r="D6" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E6" s="2">
         <v>-5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>-8</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="2">
         <v>120</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="I6" s="2">
-        <v>-0.3</v>
       </c>
       <c r="J6" s="2">
         <v>1200</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="0"/>
+        <f>C6-D6*20-E6*0.8-F6*0.6-G6*5+H6*5+I6/300</f>
         <v>0.59999999999999842</v>
       </c>
       <c r="M6" s="2">
         <v>-3</v>
       </c>
       <c r="N6" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="O6" s="2">
         <v>-13</v>
       </c>
-      <c r="O6" s="2">
-        <v>-11</v>
-      </c>
       <c r="P6" s="2">
+        <v>-10</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="S6" s="2">
         <v>70</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="S6" s="2">
-        <v>-0.1</v>
       </c>
       <c r="T6" s="2">
         <v>1300</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" si="1"/>
-        <v>12.933333333333332</v>
+        <f>M6-N6*20-O6*0.8-P6*0.6-Q6*5+R6*10+S6/300</f>
+        <v>12.333333333333332</v>
       </c>
       <c r="W6" s="2">
         <v>8</v>
       </c>
       <c r="X6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="Y6" s="2">
         <v>1055</v>
       </c>
       <c r="Z6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1455</v>
       </c>
     </row>
@@ -1618,70 +1624,70 @@
         <v>-7</v>
       </c>
       <c r="D7" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="E7" s="2">
         <v>-5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>-9</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I7" s="2">
         <v>150</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
       </c>
       <c r="J7" s="2">
         <v>1500</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="0"/>
+        <f>C7-D7*20-E7*0.8-F7*0.6-G7*5+H7*5+I7/300</f>
         <v>-1.7500000000000009</v>
       </c>
       <c r="M7" s="2">
         <v>-5</v>
       </c>
       <c r="N7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="O7" s="2">
         <v>-14</v>
       </c>
-      <c r="O7" s="2">
-        <v>-12</v>
-      </c>
       <c r="P7" s="2">
+        <v>-11</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="S7" s="2">
         <v>90</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="S7" s="2">
-        <v>-0.2</v>
       </c>
       <c r="T7" s="2">
         <v>1400</v>
       </c>
       <c r="U7" s="1">
-        <f t="shared" si="1"/>
-        <v>12.700000000000001</v>
+        <f>M7-N7*20-O7*0.8-P7*0.6-Q7*5+R7*10+S7/300</f>
+        <v>12.100000000000001</v>
       </c>
       <c r="W7" s="2">
         <v>10</v>
       </c>
       <c r="X7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="Y7" s="2">
         <v>1165</v>
       </c>
       <c r="Z7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1565</v>
       </c>
     </row>
@@ -1696,70 +1702,70 @@
         <v>-1</v>
       </c>
       <c r="D8">
-        <v>-5</v>
+        <v>0.06</v>
       </c>
       <c r="E8">
         <v>-5</v>
       </c>
       <c r="F8">
+        <v>-5</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>60</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0.06</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
       </c>
       <c r="J8">
         <v>750</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="0"/>
+        <f>C8-D8*20-E8*0.8-F8*0.6-G8*5+H8*5+I8/300</f>
         <v>5</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
       <c r="N8">
-        <v>-9</v>
+        <v>0.06</v>
       </c>
       <c r="O8">
         <v>-9</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R8">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>700</v>
       </c>
       <c r="U8" s="1">
-        <f t="shared" si="1"/>
+        <f>M8-N8*20-O8*0.8-P8*0.6-Q8*5+R8*10+S8/300</f>
         <v>12.149999999999999</v>
       </c>
       <c r="W8">
         <v>3.8</v>
       </c>
       <c r="X8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.6999999999999995E-2</v>
       </c>
       <c r="Y8">
         <v>169</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>569</v>
       </c>
     </row>
@@ -1774,70 +1780,70 @@
         <v>-1</v>
       </c>
       <c r="D9" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="6">
         <v>-3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>-2</v>
       </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
       <c r="G9" s="6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="I9" s="6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="J9" s="6">
         <v>800</v>
       </c>
       <c r="K9" s="7">
-        <f t="shared" si="0"/>
+        <f>C9-D9*20-E9*0.8-F9*0.6-G9*5+H9*5+I9/300</f>
         <v>1.3500000000000003</v>
       </c>
       <c r="M9" s="6">
         <v>-1</v>
       </c>
       <c r="N9" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="O9" s="6">
         <v>-13</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <v>-7</v>
       </c>
-      <c r="P9" s="6">
-        <v>0</v>
-      </c>
       <c r="Q9" s="6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R9" s="6">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="S9" s="6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T9" s="6">
         <v>700</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" si="1"/>
+        <f>M9-N9*20-O9*0.8-P9*0.6-Q9*5+R9*10+S9/300</f>
         <v>12.149999999999999</v>
       </c>
       <c r="W9" s="6">
         <v>3.9</v>
       </c>
       <c r="X9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.8499999999999996E-2</v>
       </c>
       <c r="Y9" s="6">
         <v>169</v>
       </c>
       <c r="Z9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>569</v>
       </c>
     </row>
@@ -1852,70 +1858,70 @@
         <v>-3</v>
       </c>
       <c r="D10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="4">
         <v>-5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>-4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I10" s="4">
         <v>25</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="4">
-        <v>-0.1</v>
       </c>
       <c r="J10" s="4">
         <v>1200</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="0"/>
+        <f>C10-D10*20-E10*0.8-F10*0.6-G10*5+H10*5+I10/300</f>
         <v>0.23333333333333323</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
       </c>
       <c r="N10" s="4">
-        <v>-11</v>
+        <v>0.12</v>
       </c>
       <c r="O10" s="4">
         <v>-10</v>
       </c>
       <c r="P10" s="4">
+        <v>-10</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>-0.05</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="S10" s="4">
         <v>40</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="R10" s="4">
-        <v>0.12</v>
-      </c>
-      <c r="S10" s="4">
-        <v>-0.05</v>
       </c>
       <c r="T10" s="4">
         <v>1000</v>
       </c>
       <c r="U10" s="1">
-        <f t="shared" si="1"/>
-        <v>12.983333333333333</v>
+        <f>M10-N10*20-O10*0.8-P10*0.6-Q10*5+R10*10+S10/300</f>
+        <v>12.183333333333332</v>
       </c>
       <c r="W10" s="4">
         <v>7.8</v>
       </c>
       <c r="X10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.11699999999999999</v>
       </c>
       <c r="Y10" s="4">
         <v>250</v>
       </c>
       <c r="Z10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>650</v>
       </c>
     </row>
@@ -1930,70 +1936,70 @@
         <v>-10</v>
       </c>
       <c r="D11" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E11" s="2">
         <v>-4</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>-8</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I11" s="2">
         <v>120</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="I11" s="2">
-        <v>-0.1</v>
       </c>
       <c r="J11" s="2">
         <v>1500</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="0"/>
+        <f>C11-D11*20-E11*0.8-F11*0.6-G11*5+H11*5+I11/300</f>
         <v>-4.950000000000002</v>
       </c>
       <c r="M11" s="2">
         <v>-4</v>
       </c>
       <c r="N11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O11" s="2">
         <v>-15</v>
       </c>
-      <c r="O11" s="2">
-        <v>-14</v>
-      </c>
       <c r="P11" s="2">
+        <v>-13</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="S11" s="2">
         <v>80</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="R11" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="S11" s="2">
-        <v>-0.1</v>
       </c>
       <c r="T11" s="2">
         <v>1500</v>
       </c>
       <c r="U11" s="1">
-        <f t="shared" si="1"/>
-        <v>13.366666666666667</v>
+        <f>M11-N11*20-O11*0.8-P11*0.6-Q11*5+R11*10+S11/300</f>
+        <v>12.766666666666667</v>
       </c>
       <c r="W11" s="2">
         <v>17</v>
       </c>
       <c r="X11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.255</v>
       </c>
       <c r="Y11" s="2">
         <v>1199</v>
       </c>
       <c r="Z11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1599</v>
       </c>
     </row>
@@ -2008,19 +2014,19 @@
         <v>-2</v>
       </c>
       <c r="D12">
-        <v>-3</v>
+        <v>0.04</v>
       </c>
       <c r="E12">
         <v>-3</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>-0.05</v>
-      </c>
-      <c r="H12">
-        <v>0.04</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2029,49 +2035,49 @@
         <v>500</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="0"/>
+        <f>C12-D12*20-E12*0.8-F12*0.6-G12*5+H12*5+I12/300</f>
         <v>1.1500000000000004</v>
       </c>
       <c r="M12">
         <v>-1</v>
       </c>
       <c r="N12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O12">
         <v>-6</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>-12</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
+        <v>0.05</v>
+      </c>
+      <c r="R12">
+        <v>0.04</v>
+      </c>
+      <c r="S12">
         <v>30</v>
-      </c>
-      <c r="Q12">
-        <v>0.04</v>
-      </c>
-      <c r="R12">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S12">
-        <v>0.05</v>
       </c>
       <c r="T12">
         <v>500</v>
       </c>
       <c r="U12" s="1">
-        <f t="shared" si="1"/>
+        <f>M12-N12*20-O12*0.8-P12*0.6-Q12*5+R12*10+S12/300</f>
         <v>9.85</v>
       </c>
       <c r="W12">
         <v>4.5999999999999996</v>
       </c>
       <c r="X12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6.8999999999999992E-2</v>
       </c>
       <c r="Y12">
         <v>138</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>538</v>
       </c>
     </row>
@@ -2086,70 +2092,70 @@
         <v>-10</v>
       </c>
       <c r="D13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E13" s="2">
         <v>-6</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>-7</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
+        <v>-0.7</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
         <v>75</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="I13" s="2">
-        <v>-0.7</v>
       </c>
       <c r="J13" s="2">
         <v>1000</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="0"/>
+        <f>C13-D13*20-E13*0.8-F13*0.6-G13*5+H13*5+I13/300</f>
         <v>-3.2499999999999991</v>
       </c>
       <c r="M13" s="2">
         <v>-6</v>
       </c>
       <c r="N13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="O13" s="2">
         <v>-11</v>
       </c>
-      <c r="O13" s="2">
-        <v>-19</v>
-      </c>
       <c r="P13" s="2">
+        <v>-18</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S13" s="2">
         <v>100</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R13" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="S13" s="2">
-        <v>-0.25</v>
       </c>
       <c r="T13" s="2">
         <v>1200</v>
       </c>
       <c r="U13" s="1">
-        <f t="shared" si="1"/>
-        <v>11.183333333333335</v>
+        <f>M13-N13*20-O13*0.8-P13*0.6-Q13*5+R13*10+S13/300</f>
+        <v>10.583333333333334</v>
       </c>
       <c r="W13" s="2">
         <v>22</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.32999999999999996</v>
       </c>
       <c r="Y13" s="2">
         <v>999</v>
       </c>
       <c r="Z13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1399</v>
       </c>
     </row>
@@ -2164,70 +2170,70 @@
         <v>-3</v>
       </c>
       <c r="D14">
-        <v>-6</v>
+        <v>0.1</v>
       </c>
       <c r="E14">
         <v>-6</v>
       </c>
       <c r="F14">
+        <v>-6</v>
+      </c>
+      <c r="G14">
+        <v>0.3</v>
+      </c>
+      <c r="H14">
+        <v>0.05</v>
+      </c>
+      <c r="I14">
         <v>10</v>
-      </c>
-      <c r="G14">
-        <v>0.05</v>
-      </c>
-      <c r="H14">
-        <v>0.1</v>
-      </c>
-      <c r="I14">
-        <v>0.3</v>
       </c>
       <c r="J14">
         <v>750</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="0"/>
+        <f>C14-D14*20-E14*0.8-F14*0.6-G14*5+H14*5+I14/300</f>
         <v>2.1833333333333336</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
+        <v>0.05</v>
+      </c>
+      <c r="O14">
         <v>-11</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>-7</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R14">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <v>400</v>
       </c>
       <c r="U14" s="1">
-        <f t="shared" si="1"/>
+        <f>M14-N14*20-O14*0.8-P14*0.6-Q14*5+R14*10+S14/300</f>
         <v>11.75</v>
       </c>
       <c r="W14">
         <v>3.2</v>
       </c>
       <c r="X14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="Y14">
         <v>47.45</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>447.45</v>
       </c>
     </row>
@@ -2242,70 +2248,70 @@
         <v>0</v>
       </c>
       <c r="D15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15">
         <v>-3</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>-4</v>
       </c>
-      <c r="F15">
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>90</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I15">
-        <v>0.1</v>
       </c>
       <c r="J15">
         <v>500</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="0"/>
+        <f>C15-D15*20-E15*0.8-F15*0.6-G15*5+H15*5+I15/300</f>
         <v>3.2</v>
       </c>
       <c r="M15">
         <v>2</v>
       </c>
       <c r="N15">
+        <v>0.04</v>
+      </c>
+      <c r="O15">
         <v>-5</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>-11</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
       <c r="Q15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R15">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>500</v>
       </c>
       <c r="U15" s="1">
-        <f t="shared" si="1"/>
+        <f>M15-N15*20-O15*0.8-P15*0.6-Q15*5+R15*10+S15/300</f>
         <v>11.3</v>
       </c>
       <c r="W15">
         <v>2.4</v>
       </c>
       <c r="X15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="Y15">
         <v>114.35</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>514.35</v>
       </c>
     </row>
@@ -2320,70 +2326,70 @@
         <v>-6</v>
       </c>
       <c r="D16" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E16" s="2">
         <v>-4</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>-8</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I16" s="2">
         <v>150</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="I16" s="2">
-        <v>-0.5</v>
       </c>
       <c r="J16" s="2">
         <v>2000</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="0"/>
+        <f>C16-D16*20-E16*0.8-F16*0.6-G16*5+H16*5+I16/300</f>
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="M16" s="2">
         <v>-5</v>
       </c>
       <c r="N16" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="O16" s="2">
         <v>-13</v>
       </c>
-      <c r="O16" s="2">
-        <v>-18</v>
-      </c>
       <c r="P16" s="2">
+        <v>-17</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="S16" s="2">
         <v>90</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="R16" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="S16" s="2">
-        <v>-0.2</v>
       </c>
       <c r="T16" s="2">
         <v>1900</v>
       </c>
       <c r="U16" s="1">
-        <f t="shared" si="1"/>
-        <v>12.7</v>
+        <f>M16-N16*20-O16*0.8-P16*0.6-Q16*5+R16*10+S16/300</f>
+        <v>12.1</v>
       </c>
       <c r="W16" s="2">
         <v>22</v>
       </c>
       <c r="X16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.32999999999999996</v>
       </c>
       <c r="Y16" s="2">
         <v>1685</v>
       </c>
       <c r="Z16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2085</v>
       </c>
     </row>
@@ -2398,70 +2404,70 @@
         <v>-1</v>
       </c>
       <c r="D17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E17">
         <v>-3</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>-4</v>
       </c>
-      <c r="F17">
+      <c r="G17">
+        <v>0.05</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>60</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I17">
-        <v>0.05</v>
       </c>
       <c r="J17">
         <v>600</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="0"/>
+        <f>C17-D17*20-E17*0.8-F17*0.6-G17*5+H17*5+I17/300</f>
         <v>2.35</v>
       </c>
       <c r="M17">
         <v>2</v>
       </c>
       <c r="N17">
-        <v>-8</v>
+        <v>0.04</v>
       </c>
       <c r="O17">
         <v>-8</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R17">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>600</v>
       </c>
       <c r="U17" s="1">
-        <f t="shared" si="1"/>
+        <f>M17-N17*20-O17*0.8-P17*0.6-Q17*5+R17*10+S17/300</f>
         <v>12.15</v>
       </c>
       <c r="W17">
         <v>2.2999999999999998</v>
       </c>
       <c r="X17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.4499999999999996E-2</v>
       </c>
       <c r="Y17">
         <v>123.75</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>523.75</v>
       </c>
     </row>
@@ -2476,70 +2482,70 @@
         <v>-6</v>
       </c>
       <c r="D18" s="2">
-        <v>-4</v>
+        <v>0.19</v>
       </c>
       <c r="E18" s="2">
         <v>-4</v>
       </c>
       <c r="F18" s="2">
+        <v>-4</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I18" s="2">
         <v>60</v>
-      </c>
-      <c r="G18" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="I18" s="2">
-        <v>-0.05</v>
       </c>
       <c r="J18" s="2">
         <v>1500</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" si="0"/>
+        <f>C18-D18*20-E18*0.8-F18*0.6-G18*5+H18*5+I18/300</f>
         <v>-3.4000000000000008</v>
       </c>
       <c r="M18" s="2">
         <v>-2</v>
       </c>
       <c r="N18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="O18" s="2">
         <v>-12</v>
       </c>
-      <c r="O18" s="2">
-        <v>-13</v>
-      </c>
       <c r="P18" s="2">
+        <v>-12</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="S18" s="2">
         <v>60</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="R18" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="S18" s="2">
-        <v>-0.1</v>
       </c>
       <c r="T18" s="2">
         <v>1800</v>
       </c>
       <c r="U18" s="1">
-        <f t="shared" si="1"/>
-        <v>12.900000000000002</v>
+        <f>M18-N18*20-O18*0.8-P18*0.6-Q18*5+R18*10+S18/300</f>
+        <v>12.3</v>
       </c>
       <c r="W18" s="2">
         <v>13.9</v>
       </c>
       <c r="X18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.20849999999999999</v>
       </c>
       <c r="Y18" s="2">
         <v>1650</v>
       </c>
       <c r="Z18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2050</v>
       </c>
     </row>
@@ -2554,70 +2560,70 @@
         <v>-10</v>
       </c>
       <c r="D19" s="2">
-        <v>-6</v>
+        <v>0.23</v>
       </c>
       <c r="E19" s="2">
         <v>-6</v>
       </c>
       <c r="F19" s="2">
+        <v>-6</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I19" s="2">
         <v>120</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="I19" s="2">
-        <v>-0.1</v>
       </c>
       <c r="J19" s="2">
         <v>2500</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="0"/>
+        <f>C19-D19*20-E19*0.8-F19*0.6-G19*5+H19*5+I19/300</f>
         <v>-4.5500000000000007</v>
       </c>
       <c r="M19" s="2">
         <v>-5</v>
       </c>
       <c r="N19" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O19" s="2">
         <v>-15</v>
       </c>
-      <c r="O19" s="2">
-        <v>-16</v>
-      </c>
       <c r="P19" s="2">
+        <v>-15</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>-0.15</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="S19" s="2">
         <v>90</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="R19" s="2">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="S19" s="2">
-        <v>-0.15</v>
       </c>
       <c r="T19" s="2">
         <v>2000</v>
       </c>
       <c r="U19" s="1">
-        <f t="shared" si="1"/>
-        <v>13.049999999999999</v>
+        <f>M19-N19*20-O19*0.8-P19*0.6-Q19*5+R19*10+S19/300</f>
+        <v>12.45</v>
       </c>
       <c r="W19" s="2">
         <v>19.2</v>
       </c>
       <c r="X19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.28799999999999998</v>
       </c>
       <c r="Y19" s="2">
         <v>1800</v>
       </c>
       <c r="Z19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2200</v>
       </c>
     </row>
@@ -2626,20 +2632,20 @@
         <v>91</v>
       </c>
       <c r="K20" s="1">
-        <f>C20-H20*20-D20*0.8-E20*0.6-I20*5+G20*5+F20/300</f>
+        <f>C20-D20*20-E20*0.8-F20*0.6-G20*5+H20*5+I20/300</f>
         <v>0</v>
       </c>
       <c r="M20">
         <v>1</v>
       </c>
-      <c r="R20">
+      <c r="N20">
         <v>0.03</v>
       </c>
       <c r="T20">
         <v>500</v>
       </c>
       <c r="U20" s="1">
-        <f t="shared" si="1"/>
+        <f>M20-N20*20-O20*0.8-P20*0.6-Q20*5+R20*10+S20/300</f>
         <v>0.4</v>
       </c>
       <c r="X20">
@@ -2656,20 +2662,20 @@
         <v>92</v>
       </c>
       <c r="K21" s="1">
-        <f>C21-H21*20-D21*0.8-E21*0.6-I21*5+G21*5+F21/300</f>
+        <f>C21-D21*20-E21*0.8-F21*0.6-G21*5+H21*5+I21/300</f>
         <v>0</v>
       </c>
       <c r="M21">
         <v>1</v>
       </c>
-      <c r="R21">
+      <c r="N21">
         <v>0.04</v>
       </c>
       <c r="T21">
         <v>500</v>
       </c>
       <c r="U21" s="1">
-        <f t="shared" si="1"/>
+        <f>M21-N21*20-O21*0.8-P21*0.6-Q21*5+R21*10+S21/300</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="X21">
@@ -2692,70 +2698,70 @@
         <v>-2</v>
       </c>
       <c r="D22">
+        <v>0.1</v>
+      </c>
+      <c r="E22">
         <v>-4</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>-3</v>
       </c>
-      <c r="F22">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I22">
         <v>100</v>
-      </c>
-      <c r="G22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H22">
-        <v>0.1</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
       </c>
       <c r="J22">
         <v>400</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="0"/>
+        <f>C22-D22*20-E22*0.8-F22*0.6-G22*5+H22*5+I22/300</f>
         <v>1.6833333333333333</v>
       </c>
       <c r="M22">
         <v>1</v>
       </c>
       <c r="N22">
+        <v>0.1</v>
+      </c>
+      <c r="O22">
         <v>-4</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>-14</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0.06</v>
+      </c>
+      <c r="S22">
         <v>40</v>
-      </c>
-      <c r="Q22">
-        <v>0.06</v>
-      </c>
-      <c r="R22">
-        <v>0.1</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
       </c>
       <c r="T22">
         <v>300</v>
       </c>
       <c r="U22" s="1">
-        <f t="shared" si="1"/>
+        <f>M22-N22*20-O22*0.8-P22*0.6-Q22*5+R22*10+S22/300</f>
         <v>11.333333333333334</v>
       </c>
       <c r="W22">
         <v>7.2</v>
       </c>
       <c r="X22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.108</v>
       </c>
       <c r="Y22">
         <v>25.95</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>425.95</v>
       </c>
     </row>
@@ -2770,70 +2776,70 @@
         <v>-2</v>
       </c>
       <c r="D23">
-        <v>-4</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E23">
         <v>-4</v>
       </c>
       <c r="F23">
+        <v>-4</v>
+      </c>
+      <c r="G23">
+        <v>0.05</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>100</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I23">
-        <v>0.05</v>
-      </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="0"/>
+        <f>C23-D23*20-E23*0.8-F23*0.6-G23*5+H23*5+I23/300</f>
         <v>2.2833333333333332</v>
       </c>
       <c r="M23">
         <v>2</v>
       </c>
       <c r="N23">
-        <v>-5</v>
+        <v>0.03</v>
       </c>
       <c r="O23">
         <v>-5</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R23">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="S23">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="T23">
         <v>0</v>
       </c>
       <c r="U23" s="1">
-        <f t="shared" si="1"/>
+        <f>M23-N23*20-O23*0.8-P23*0.6-Q23*5+R23*10+S23/300</f>
         <v>7.9</v>
       </c>
       <c r="W23">
         <v>1.9</v>
       </c>
       <c r="X23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.8499999999999998E-2</v>
       </c>
       <c r="Y23">
         <v>8.99</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>408.99</v>
       </c>
     </row>
@@ -2848,70 +2854,70 @@
         <v>-7</v>
       </c>
       <c r="D24" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E24" s="2">
         <v>-6</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>-7</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I24" s="2">
         <v>140</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I24" s="2">
-        <v>-0.3</v>
       </c>
       <c r="J24" s="2">
         <v>2000</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="0"/>
+        <f>C24-D24*20-E24*0.8-F24*0.6-G24*5+H24*5+I24/300</f>
         <v>-0.88333333333333386</v>
       </c>
       <c r="M24" s="2">
         <v>-5</v>
       </c>
       <c r="N24" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="O24" s="2">
         <v>-12</v>
       </c>
-      <c r="O24" s="2">
-        <v>-14</v>
-      </c>
       <c r="P24" s="2">
+        <v>-13</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S24" s="2">
         <v>100</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R24" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="S24" s="2">
-        <v>-0.2</v>
       </c>
       <c r="T24" s="2">
         <v>1300</v>
       </c>
       <c r="U24" s="1">
-        <f t="shared" si="1"/>
-        <v>11.933333333333335</v>
+        <f>M24-N24*20-O24*0.8-P24*0.6-Q24*5+R24*10+S24/300</f>
+        <v>11.333333333333336</v>
       </c>
       <c r="W24" s="2">
         <v>12.8</v>
       </c>
       <c r="X24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.192</v>
       </c>
       <c r="Y24" s="2">
         <v>999</v>
       </c>
       <c r="Z24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1399</v>
       </c>
     </row>
@@ -2926,67 +2932,67 @@
         <v>-2</v>
       </c>
       <c r="D25">
-        <v>-2</v>
+        <v>0.12</v>
       </c>
       <c r="E25">
         <v>-2</v>
       </c>
       <c r="F25">
+        <v>-2</v>
+      </c>
+      <c r="G25">
+        <v>0.15</v>
+      </c>
+      <c r="H25">
+        <v>0.05</v>
+      </c>
+      <c r="I25">
         <v>80</v>
-      </c>
-      <c r="G25">
-        <v>0.05</v>
-      </c>
-      <c r="H25">
-        <v>0.12</v>
-      </c>
-      <c r="I25">
-        <v>0.15</v>
       </c>
       <c r="J25">
         <v>1000</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="0"/>
+        <f>C25-D25*20-E25*0.8-F25*0.6-G25*5+H25*5+I25/300</f>
         <v>-1.8333333333333339</v>
       </c>
       <c r="M25">
         <v>-2</v>
       </c>
       <c r="N25">
-        <v>-2</v>
+        <v>0.16</v>
       </c>
       <c r="O25">
         <v>-2</v>
       </c>
       <c r="P25">
+        <v>-2</v>
+      </c>
+      <c r="Q25">
+        <v>0.24</v>
+      </c>
+      <c r="R25">
+        <v>0.08</v>
+      </c>
+      <c r="S25">
         <v>80</v>
-      </c>
-      <c r="Q25">
-        <v>0.08</v>
-      </c>
-      <c r="R25">
-        <v>0.16</v>
-      </c>
-      <c r="S25">
-        <v>0.24</v>
       </c>
       <c r="T25">
         <v>600</v>
       </c>
       <c r="U25" s="1">
-        <f t="shared" si="1"/>
+        <f>M25-N25*20-O25*0.8-P25*0.6-Q25*5+R25*10+S25/300</f>
         <v>-2.5333333333333341</v>
       </c>
       <c r="X25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y25">
         <v>59.99</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>459.99</v>
       </c>
     </row>
@@ -3001,67 +3007,67 @@
         <v>-1.5</v>
       </c>
       <c r="D26">
-        <v>-1</v>
+        <v>0.09</v>
       </c>
       <c r="E26">
         <v>-1</v>
       </c>
       <c r="F26">
+        <v>-1</v>
+      </c>
+      <c r="G26">
+        <v>0.1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>60</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0.09</v>
-      </c>
-      <c r="I26">
-        <v>0.1</v>
       </c>
       <c r="J26">
         <v>750</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="0"/>
+        <f>C26-D26*20-E26*0.8-F26*0.6-G26*5+H26*5+I26/300</f>
         <v>-2.1999999999999997</v>
       </c>
       <c r="M26">
         <v>-1</v>
       </c>
       <c r="N26">
-        <v>-1</v>
+        <v>0.08</v>
       </c>
       <c r="O26">
         <v>-1</v>
       </c>
       <c r="P26">
+        <v>-1</v>
+      </c>
+      <c r="Q26">
+        <v>0.12</v>
+      </c>
+      <c r="R26">
+        <v>0.04</v>
+      </c>
+      <c r="S26">
         <v>40</v>
-      </c>
-      <c r="Q26">
-        <v>0.04</v>
-      </c>
-      <c r="R26">
-        <v>0.08</v>
-      </c>
-      <c r="S26">
-        <v>0.12</v>
       </c>
       <c r="T26">
         <v>500</v>
       </c>
       <c r="U26" s="1">
-        <f t="shared" si="1"/>
+        <f>M26-N26*20-O26*0.8-P26*0.6-Q26*5+R26*10+S26/300</f>
         <v>-1.2666666666666671</v>
       </c>
       <c r="X26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y26">
         <v>44.99</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>444.99</v>
       </c>
     </row>
@@ -3076,67 +3082,67 @@
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0.05</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <v>40</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0.06</v>
-      </c>
-      <c r="I27">
-        <v>0.05</v>
       </c>
       <c r="J27">
         <v>500</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="0"/>
+        <f>C27-D27*20-E27*0.8-F27*0.6-G27*5+H27*5+I27/300</f>
         <v>-2.3166666666666669</v>
       </c>
       <c r="M27">
         <v>-0.5</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0.06</v>
+      </c>
+      <c r="R27">
+        <v>0.02</v>
+      </c>
+      <c r="S27">
         <v>20</v>
-      </c>
-      <c r="Q27">
-        <v>0.02</v>
-      </c>
-      <c r="R27">
-        <v>0.04</v>
-      </c>
-      <c r="S27">
-        <v>0.06</v>
       </c>
       <c r="T27">
         <v>400</v>
       </c>
       <c r="U27" s="1">
-        <f t="shared" si="1"/>
+        <f>M27-N27*20-O27*0.8-P27*0.6-Q27*5+R27*10+S27/300</f>
         <v>-1.3333333333333335</v>
       </c>
       <c r="X27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y27">
         <v>29.99</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>429.99</v>
       </c>
     </row>
@@ -3151,64 +3157,64 @@
         <v>-1</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
         <v>2</v>
       </c>
-      <c r="F28">
+      <c r="G28">
+        <v>0.1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <v>5</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0.03</v>
-      </c>
-      <c r="I28">
-        <v>0.1</v>
       </c>
       <c r="J28">
         <v>300</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="0"/>
+        <f>C28-D28*20-E28*0.8-F28*0.6-G28*5+H28*5+I28/300</f>
         <v>-3.2833333333333332</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
+        <v>0.03</v>
+      </c>
+      <c r="O28">
         <v>-3</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>-4</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
+        <v>0.05</v>
+      </c>
+      <c r="R28">
+        <v>0.02</v>
+      </c>
+      <c r="S28">
         <v>20</v>
-      </c>
-      <c r="Q28">
-        <v>0.02</v>
-      </c>
-      <c r="R28">
-        <v>0.03</v>
-      </c>
-      <c r="S28">
-        <v>0.05</v>
       </c>
       <c r="T28">
         <v>300</v>
       </c>
       <c r="U28" s="1">
+        <f>M28-N28*20-O28*0.8-P28*0.6-Q28*5+R28*10+S28/300</f>
+        <v>4.2166666666666668</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z28">
         <f t="shared" si="1"/>
-        <v>4.2166666666666668</v>
-      </c>
-      <c r="X28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
@@ -3223,70 +3229,70 @@
         <v>-16</v>
       </c>
       <c r="D29" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="2">
         <v>-6</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>-12</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="2">
         <v>200</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="I29" s="2">
-        <v>-0.3</v>
       </c>
       <c r="J29" s="2">
         <v>1500</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="0"/>
+        <f>C29-D29*20-E29*0.8-F29*0.6-G29*5+H29*5+I29/300</f>
         <v>-7.333333333333333</v>
       </c>
       <c r="M29" s="2">
         <v>-5</v>
       </c>
       <c r="N29" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="O29" s="2">
         <v>-16</v>
       </c>
-      <c r="O29" s="2">
-        <v>-11</v>
-      </c>
       <c r="P29" s="2">
+        <v>-10</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>-0.15</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="S29" s="2">
         <v>90</v>
-      </c>
-      <c r="Q29" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="R29" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="S29" s="2">
-        <v>-0.15</v>
       </c>
       <c r="T29" s="2">
         <v>1400</v>
       </c>
       <c r="U29" s="1">
-        <f t="shared" si="1"/>
-        <v>11.85</v>
+        <f>M29-N29*20-O29*0.8-P29*0.6-Q29*5+R29*10+S29/300</f>
+        <v>11.25</v>
       </c>
       <c r="W29" s="2">
         <v>17.399999999999999</v>
       </c>
       <c r="X29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.26099999999999995</v>
       </c>
       <c r="Y29" s="2">
         <v>1099</v>
       </c>
       <c r="Z29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1499</v>
       </c>
     </row>
@@ -3301,70 +3307,70 @@
         <v>-1</v>
       </c>
       <c r="D30">
+        <v>0.04</v>
+      </c>
+      <c r="E30">
         <v>-3</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>-1</v>
       </c>
-      <c r="F30">
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>5</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0.04</v>
-      </c>
-      <c r="I30">
-        <v>0.1</v>
       </c>
       <c r="J30">
         <v>300</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="0"/>
+        <f>C30-D30*20-E30*0.8-F30*0.6-G30*5+H30*5+I30/300</f>
         <v>0.7166666666666669</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30">
+        <v>0.05</v>
+      </c>
+      <c r="O30">
         <v>-12</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>-6</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
       <c r="Q30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R30">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="S30">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="T30">
         <v>500</v>
       </c>
       <c r="U30" s="1">
-        <f t="shared" si="1"/>
+        <f>M30-N30*20-O30*0.8-P30*0.6-Q30*5+R30*10+S30/300</f>
         <v>11.700000000000001</v>
       </c>
       <c r="W30">
         <v>3.84</v>
       </c>
       <c r="X30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.7599999999999998E-2</v>
       </c>
       <c r="Y30">
         <v>151</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>551</v>
       </c>
     </row>
@@ -3379,70 +3385,70 @@
         <v>-11</v>
       </c>
       <c r="D31" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="E31" s="2">
         <v>-3</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>-9</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I31" s="2">
         <v>100</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0</v>
       </c>
       <c r="J31" s="2">
         <v>1300</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="0"/>
+        <f>C31-D31*20-E31*0.8-F31*0.6-G31*5+H31*5+I31/300</f>
         <v>-6.666666666666667</v>
       </c>
       <c r="M31" s="2">
         <v>-6</v>
       </c>
       <c r="N31" s="2">
-        <v>-15</v>
+        <v>0.25</v>
       </c>
       <c r="O31" s="2">
         <v>-15</v>
       </c>
       <c r="P31" s="2">
+        <v>-15</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="R31" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="S31" s="2">
         <v>90</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="R31" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="S31" s="2">
-        <v>-0.1</v>
       </c>
       <c r="T31" s="2">
         <v>1200</v>
       </c>
       <c r="U31" s="1">
-        <f t="shared" si="1"/>
+        <f>M31-N31*20-O31*0.8-P31*0.6-Q31*5+R31*10+S31/300</f>
         <v>12.4</v>
       </c>
       <c r="W31" s="2">
         <v>16.760000000000002</v>
       </c>
       <c r="X31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.25140000000000001</v>
       </c>
       <c r="Y31" s="2">
         <v>899.99</v>
       </c>
       <c r="Z31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1299.99</v>
       </c>
     </row>
@@ -3457,67 +3463,67 @@
         <v>-2</v>
       </c>
       <c r="D32">
+        <v>0.05</v>
+      </c>
+      <c r="E32">
         <v>-5</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>-6</v>
       </c>
-      <c r="F32">
+      <c r="G32">
+        <v>0.2</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
         <v>50</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0.05</v>
-      </c>
-      <c r="I32">
-        <v>0.2</v>
       </c>
       <c r="J32">
         <v>750</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="0"/>
+        <f>C32-D32*20-E32*0.8-F32*0.6-G32*5+H32*5+I32/300</f>
         <v>3.7666666666666662</v>
       </c>
       <c r="M32">
         <v>-1</v>
       </c>
       <c r="N32">
+        <v>0.06</v>
+      </c>
+      <c r="O32">
         <v>-14</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>-6</v>
       </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
       <c r="Q32">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R32">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="S32">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="T32">
         <v>400</v>
       </c>
       <c r="U32" s="1">
-        <f t="shared" si="1"/>
+        <f>M32-N32*20-O32*0.8-P32*0.6-Q32*5+R32*10+S32/300</f>
         <v>12.1</v>
       </c>
       <c r="W32">
         <v>4.4000000000000004</v>
       </c>
       <c r="X32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
@@ -3532,70 +3538,70 @@
         <v>-0.5</v>
       </c>
       <c r="D33">
-        <v>-5</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E33">
         <v>-5</v>
       </c>
       <c r="F33">
-        <v>30</v>
+        <v>-5</v>
       </c>
       <c r="G33">
         <v>0.05</v>
       </c>
       <c r="H33">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I33">
-        <v>0.05</v>
+        <v>30</v>
       </c>
       <c r="J33">
         <v>1000</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="0"/>
+        <f>C33-D33*20-E33*0.8-F33*0.6-G33*5+H33*5+I33/300</f>
         <v>5.1999999999999993</v>
       </c>
       <c r="M33">
         <v>1</v>
       </c>
       <c r="N33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O33">
         <v>-7</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>-12</v>
       </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
       <c r="Q33">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R33">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="S33">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T33">
         <v>500</v>
       </c>
       <c r="U33" s="1">
-        <f t="shared" si="1"/>
+        <f>M33-N33*20-O33*0.8-P33*0.6-Q33*5+R33*10+S33/300</f>
         <v>12.149999999999999</v>
       </c>
       <c r="W33">
         <v>4.8</v>
       </c>
       <c r="X33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="Y33">
         <v>64.989999999999995</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>464.99</v>
       </c>
     </row>
@@ -3610,64 +3616,64 @@
         <v>-6.5</v>
       </c>
       <c r="D34" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="E34" s="2">
         <v>-6</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>-10</v>
       </c>
-      <c r="F34" s="2">
+      <c r="G34" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I34" s="2">
         <v>250</v>
-      </c>
-      <c r="G34" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H34" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="I34" s="2">
-        <v>-0.5</v>
       </c>
       <c r="J34" s="2">
         <v>2000</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="0"/>
+        <f>C34-D34*20-E34*0.8-F34*0.6-G34*5+H34*5+I34/300</f>
         <v>2.7333333333333338</v>
       </c>
       <c r="M34" s="2">
         <v>-2</v>
       </c>
       <c r="N34" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="O34" s="2">
         <v>-10</v>
       </c>
-      <c r="O34" s="2">
-        <v>-16</v>
-      </c>
       <c r="P34" s="2">
+        <v>-15</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="R34" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="S34" s="2">
         <v>50</v>
-      </c>
-      <c r="Q34" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="R34" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="S34" s="2">
-        <v>-0.05</v>
       </c>
       <c r="T34" s="2">
         <v>1500</v>
       </c>
       <c r="U34" s="1">
+        <f>M34-N34*20-O34*0.8-P34*0.6-Q34*5+R34*10+S34/300</f>
+        <v>10.816666666666666</v>
+      </c>
+      <c r="X34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z34" s="2">
         <f t="shared" si="1"/>
-        <v>11.416666666666666</v>
-      </c>
-      <c r="X34" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z34" s="2">
-        <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
@@ -3682,70 +3688,70 @@
         <v>-8</v>
       </c>
       <c r="D35" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="E35" s="2">
         <v>-6</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>-12</v>
       </c>
-      <c r="F35" s="2">
+      <c r="G35" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I35" s="2">
         <v>400</v>
-      </c>
-      <c r="G35" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="H35" s="2">
-        <v>0.32</v>
-      </c>
-      <c r="I35" s="2">
-        <v>-0.5</v>
       </c>
       <c r="J35" s="2">
         <v>2000</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="0"/>
+        <f>C35-D35*20-E35*0.8-F35*0.6-G35*5+H35*5+I35/300</f>
         <v>2.4333333333333327</v>
       </c>
       <c r="M35" s="2">
         <v>-4</v>
       </c>
       <c r="N35" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="O35" s="2">
         <v>-12</v>
       </c>
-      <c r="O35" s="2">
-        <v>-17</v>
-      </c>
       <c r="P35" s="2">
+        <v>-16</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="S35" s="2">
         <v>70</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="R35" s="2">
-        <v>0.32</v>
-      </c>
-      <c r="S35" s="2">
-        <v>-0.1</v>
       </c>
       <c r="T35" s="2">
         <v>1600</v>
       </c>
       <c r="U35" s="1">
-        <f t="shared" si="1"/>
-        <v>11.333333333333332</v>
+        <f>M35-N35*20-O35*0.8-P35*0.6-Q35*5+R35*10+S35/300</f>
+        <v>10.733333333333333</v>
       </c>
       <c r="W35" s="2">
         <v>22.2</v>
       </c>
       <c r="X35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.33299999999999996</v>
       </c>
       <c r="Y35" s="2">
         <v>797.99</v>
       </c>
       <c r="Z35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1197.99</v>
       </c>
     </row>
@@ -3761,42 +3767,42 @@
         <v>-1</v>
       </c>
       <c r="N36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O36">
         <v>-12</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>-9</v>
       </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
       <c r="Q36">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R36">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="S36">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="T36">
         <v>600</v>
       </c>
       <c r="U36" s="1">
-        <f t="shared" si="1"/>
+        <f>M36-N36*20-O36*0.8-P36*0.6-Q36*5+R36*10+S36/300</f>
         <v>12.100000000000001</v>
       </c>
       <c r="W36">
         <v>3.8</v>
       </c>
       <c r="X36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.6999999999999995E-2</v>
       </c>
       <c r="Y36">
         <v>200</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
@@ -3811,42 +3817,42 @@
         <v>-1</v>
       </c>
       <c r="N37">
+        <v>0.05</v>
+      </c>
+      <c r="O37">
         <v>-9</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>-12</v>
       </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
       <c r="Q37">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R37">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="T37">
         <v>500</v>
       </c>
       <c r="U37" s="1">
-        <f t="shared" si="1"/>
+        <f>M37-N37*20-O37*0.8-P37*0.6-Q37*5+R37*10+S37/300</f>
         <v>12.149999999999999</v>
       </c>
       <c r="W37">
         <v>3.6</v>
       </c>
       <c r="X37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="Y37">
         <v>43.95</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>443.95</v>
       </c>
     </row>
@@ -3861,41 +3867,41 @@
         <v>0</v>
       </c>
       <c r="N38" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O38" s="4">
         <v>-9</v>
       </c>
-      <c r="O38" s="4">
+      <c r="P38" s="4">
         <v>-13</v>
       </c>
-      <c r="P38" s="4">
+      <c r="Q38" s="4">
+        <v>-0.05</v>
+      </c>
+      <c r="R38" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="S38" s="4">
         <v>20</v>
-      </c>
-      <c r="Q38" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="R38" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="S38" s="4">
-        <v>-0.05</v>
       </c>
       <c r="T38" s="4">
         <v>1000</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="1"/>
+        <f>M38-N38*20-O38*0.8-P38*0.6-Q38*5+R38*10+S38/300</f>
         <v>12.716666666666665</v>
       </c>
       <c r="W38" s="4">
         <v>9.5</v>
       </c>
       <c r="X38" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.14249999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="U39" s="1">
-        <f t="shared" si="1"/>
+        <f>M39-N39*20-O39*0.8-P39*0.6-Q39*5+R39*10+S39/300</f>
         <v>0</v>
       </c>
     </row>
@@ -3910,56 +3916,56 @@
         <v>-2</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="E40">
         <v>5</v>
       </c>
       <c r="F40">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>0.1</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
         <v>-50</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0.05</v>
-      </c>
-      <c r="I40">
-        <v>0.1</v>
       </c>
       <c r="J40">
         <v>1500</v>
       </c>
       <c r="K40" s="1">
-        <f>C40-H40*20-D40*0.8-E40*0.6-I40*5+G40*5+F40/300</f>
+        <f>C40-D40*20-E40*0.8-F40*0.6-G40*5+H40*5+I40/300</f>
         <v>-10.666666666666666</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="O40">
         <v>0</v>
       </c>
       <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0.1</v>
+      </c>
+      <c r="R40">
+        <v>0.02</v>
+      </c>
+      <c r="S40">
         <v>30</v>
-      </c>
-      <c r="Q40">
-        <v>0.02</v>
-      </c>
-      <c r="R40">
-        <v>0.04</v>
-      </c>
-      <c r="S40">
-        <v>0.1</v>
       </c>
       <c r="T40">
         <v>1500</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="1"/>
+        <f>M40-N40*20-O40*0.8-P40*0.6-Q40*5+R40*10+S40/300</f>
         <v>-1</v>
       </c>
       <c r="X40">
@@ -3982,50 +3988,50 @@
         <v>-2</v>
       </c>
       <c r="D41">
+        <v>0.05</v>
+      </c>
+      <c r="E41">
         <v>-6</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>-5</v>
       </c>
-      <c r="F41">
-        <v>50</v>
-      </c>
       <c r="G41">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>0.05</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K41" s="1">
-        <f>C41-H41*20-D41*0.8-E41*0.6-I41*5+G41*5+F41/300</f>
+        <f>C41-D41*20-E41*0.8-F41*0.6-G41*5+H41*5+I41/300</f>
         <v>5.2166666666666677</v>
       </c>
       <c r="M41">
         <v>1</v>
       </c>
       <c r="N41">
+        <v>0.05</v>
+      </c>
+      <c r="O41">
         <v>-9</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>-7</v>
       </c>
-      <c r="P41">
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0.02</v>
+      </c>
+      <c r="S41">
         <v>50</v>
       </c>
-      <c r="Q41">
-        <v>0.02</v>
-      </c>
-      <c r="R41">
-        <v>0.05</v>
-      </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
       <c r="U41" s="1">
-        <f t="shared" si="1"/>
+        <f>M41-N41*20-O41*0.8-P41*0.6-Q41*5+R41*10+S41/300</f>
         <v>11.766666666666666</v>
       </c>
       <c r="X41">
@@ -4048,56 +4054,56 @@
         <v>-2</v>
       </c>
       <c r="D42">
+        <v>0.06</v>
+      </c>
+      <c r="E42">
         <v>-8</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>-3</v>
       </c>
-      <c r="F42">
+      <c r="G42">
+        <v>0.05</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
         <v>120</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0.06</v>
-      </c>
-      <c r="I42">
-        <v>0.05</v>
       </c>
       <c r="J42">
         <v>500</v>
       </c>
       <c r="K42" s="1">
-        <f>C42-H42*20-D42*0.8-E42*0.6-I42*5+G42*5+F42/300</f>
+        <f>C42-D42*20-E42*0.8-F42*0.6-G42*5+H42*5+I42/300</f>
         <v>5.15</v>
       </c>
       <c r="M42">
         <v>1</v>
       </c>
       <c r="N42">
+        <v>0.06</v>
+      </c>
+      <c r="O42">
         <v>-8</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>-9</v>
       </c>
-      <c r="P42">
+      <c r="Q42">
+        <v>0.05</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
         <v>60</v>
-      </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42">
-        <v>0.06</v>
-      </c>
-      <c r="S42">
-        <v>0.05</v>
       </c>
       <c r="T42">
         <v>500</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="U42:U44" si="2">M42-N42*20-O42*0.8-P42*0.6-Q42*5+R42*10+S42/300</f>
         <v>11.549999999999999</v>
       </c>
       <c r="X42">
@@ -4120,19 +4126,19 @@
         <v>-1</v>
       </c>
       <c r="D43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E43">
         <v>-5</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>-7</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -4141,26 +4147,26 @@
         <v>750</v>
       </c>
       <c r="K43" s="1">
-        <f>C43-H43*20-D43*0.8-E43*0.6-I43*5+G43*5+F43/300</f>
+        <f>C43-D43*20-E43*0.8-F43*0.6-G43*5+H43*5+I43/300</f>
         <v>5.8</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O43">
         <v>-9</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>-10</v>
       </c>
-      <c r="P43">
-        <v>0</v>
-      </c>
       <c r="Q43">
         <v>0</v>
       </c>
       <c r="R43">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="S43">
         <v>0</v>
@@ -4169,7 +4175,7 @@
         <v>750</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.8</v>
       </c>
       <c r="X43">
@@ -4182,7 +4188,41 @@
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U44" s="1"/>
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="K44" s="1"/>
+      <c r="M44">
+        <v>-2</v>
+      </c>
+      <c r="N44">
+        <v>0.22</v>
+      </c>
+      <c r="O44">
+        <v>-10</v>
+      </c>
+      <c r="P44">
+        <v>-15</v>
+      </c>
+      <c r="Q44">
+        <v>-0.1</v>
+      </c>
+      <c r="R44">
+        <v>0.08</v>
+      </c>
+      <c r="S44">
+        <v>65</v>
+      </c>
+      <c r="T44">
+        <v>1800</v>
+      </c>
+      <c r="U44" s="1">
+        <f t="shared" si="2"/>
+        <v>12.116666666666667</v>
+      </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="U45" s="1"/>

</xml_diff>

<commit_message>
-4 -4 556 muzzles
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59136AD6-17C9-4021-8755-EC0B70429D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89345487-2219-4402-8225-DB8C2CC9C189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,10 +1343,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O3">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="P3">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="Q3">
         <v>0.05</v>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="U3" s="1">
         <f t="shared" ref="U3:U41" si="1">M3-N3*20-O3*0.8-P3*0.6-Q3*5+R3*10+S3/300</f>
-        <v>11.75</v>
+        <v>17.350000000000001</v>
       </c>
       <c r="W3">
         <v>4.8</v>
@@ -1421,10 +1421,10 @@
         <v>0.05</v>
       </c>
       <c r="O4">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="P4">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="Q4">
         <v>0.1</v>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="U4" s="1">
         <f t="shared" si="1"/>
-        <v>11.3</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="W4">
         <v>3.8</v>
@@ -1499,10 +1499,10 @@
         <v>0.09</v>
       </c>
       <c r="O5" s="2">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="P5" s="2">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="Q5" s="2">
         <v>-0.05</v>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="U5" s="1">
         <f t="shared" si="1"/>
-        <v>12.216666666666667</v>
+        <v>17.816666666666666</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
@@ -1577,10 +1577,10 @@
         <v>0.12</v>
       </c>
       <c r="O6" s="2">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="P6" s="2">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="Q6" s="2">
         <v>-0.1</v>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>12.333333333333332</v>
+        <v>17.933333333333337</v>
       </c>
       <c r="W6" s="2">
         <v>8</v>
@@ -1655,10 +1655,10 @@
         <v>0.15</v>
       </c>
       <c r="O7" s="2">
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="P7" s="2">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="Q7" s="2">
         <v>-0.2</v>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>12.100000000000001</v>
+        <v>17.7</v>
       </c>
       <c r="W7" s="2">
         <v>10</v>
@@ -1733,10 +1733,10 @@
         <v>0.06</v>
       </c>
       <c r="O8">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="P8">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="Q8">
         <v>0.05</v>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="U8" s="1">
         <f t="shared" si="1"/>
-        <v>12.149999999999999</v>
+        <v>17.75</v>
       </c>
       <c r="W8">
         <v>3.8</v>
@@ -1811,10 +1811,10 @@
         <v>0.06</v>
       </c>
       <c r="O9" s="6">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="P9" s="6">
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="Q9" s="6">
         <v>0.05</v>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="U9" s="1">
         <f t="shared" si="1"/>
-        <v>12.149999999999999</v>
+        <v>17.75</v>
       </c>
       <c r="W9" s="6">
         <v>3.9</v>
@@ -1889,10 +1889,10 @@
         <v>0.12</v>
       </c>
       <c r="O10" s="4">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="P10" s="4">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="Q10" s="4">
         <v>-0.05</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>12.183333333333332</v>
+        <v>17.783333333333335</v>
       </c>
       <c r="W10" s="4">
         <v>7.8</v>
@@ -1967,10 +1967,10 @@
         <v>0.25</v>
       </c>
       <c r="O11" s="2">
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="P11" s="2">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="Q11" s="2">
         <v>-0.1</v>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="U11" s="1">
         <f t="shared" si="1"/>
-        <v>12.766666666666667</v>
+        <v>18.366666666666664</v>
       </c>
       <c r="W11" s="2">
         <v>17</v>
@@ -2045,10 +2045,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O12">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="P12">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="Q12">
         <v>0.05</v>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="U12" s="1">
         <f t="shared" si="1"/>
-        <v>9.85</v>
+        <v>15.45</v>
       </c>
       <c r="W12">
         <v>4.5999999999999996</v>
@@ -2123,10 +2123,10 @@
         <v>0.3</v>
       </c>
       <c r="O13" s="2">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="P13" s="2">
-        <v>-18</v>
+        <v>-22</v>
       </c>
       <c r="Q13" s="2">
         <v>-0.25</v>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>10.583333333333334</v>
+        <v>16.183333333333334</v>
       </c>
       <c r="W13" s="2">
         <v>22</v>
@@ -2201,10 +2201,10 @@
         <v>0.05</v>
       </c>
       <c r="O14">
+        <v>-15</v>
+      </c>
+      <c r="P14">
         <v>-11</v>
-      </c>
-      <c r="P14">
-        <v>-7</v>
       </c>
       <c r="Q14">
         <v>0.05</v>
@@ -2220,7 +2220,7 @@
       </c>
       <c r="U14" s="1">
         <f t="shared" si="1"/>
-        <v>11.75</v>
+        <v>17.350000000000001</v>
       </c>
       <c r="W14">
         <v>3.2</v>
@@ -2279,10 +2279,10 @@
         <v>0.04</v>
       </c>
       <c r="O15">
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="P15">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="Q15">
         <v>0.1</v>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="U15" s="1">
         <f t="shared" si="1"/>
-        <v>11.3</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="W15">
         <v>2.4</v>
@@ -2357,10 +2357,10 @@
         <v>0.3</v>
       </c>
       <c r="O16" s="2">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="P16" s="2">
-        <v>-17</v>
+        <v>-21</v>
       </c>
       <c r="Q16" s="2">
         <v>-0.2</v>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>12.1</v>
+        <v>17.700000000000003</v>
       </c>
       <c r="W16" s="2">
         <v>22</v>
@@ -2435,10 +2435,10 @@
         <v>0.04</v>
       </c>
       <c r="O17">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="P17">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="Q17">
         <v>0.05</v>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="U17" s="1">
         <f t="shared" si="1"/>
-        <v>12.15</v>
+        <v>17.75</v>
       </c>
       <c r="W17">
         <v>2.2999999999999998</v>
@@ -2513,10 +2513,10 @@
         <v>0.2</v>
       </c>
       <c r="O18" s="2">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="P18" s="2">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="Q18" s="2">
         <v>-0.1</v>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>12.3</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="W18" s="2">
         <v>13.9</v>
@@ -2591,10 +2591,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="O19" s="2">
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="P19" s="2">
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="Q19" s="2">
         <v>-0.15</v>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>12.45</v>
+        <v>18.05</v>
       </c>
       <c r="W19" s="2">
         <v>19.2</v>
@@ -2729,10 +2729,10 @@
         <v>0.1</v>
       </c>
       <c r="O22">
-        <v>-4</v>
+        <v>-8</v>
       </c>
       <c r="P22">
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="U22" s="1">
         <f t="shared" si="1"/>
-        <v>11.333333333333334</v>
+        <v>16.933333333333334</v>
       </c>
       <c r="W22">
         <v>7.2</v>
@@ -2807,10 +2807,10 @@
         <v>0.03</v>
       </c>
       <c r="O23">
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="P23">
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="Q23">
         <v>0.1</v>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="U23" s="1">
         <f t="shared" si="1"/>
-        <v>7.9</v>
+        <v>13.5</v>
       </c>
       <c r="W23">
         <v>1.9</v>
@@ -2885,10 +2885,10 @@
         <v>0.19</v>
       </c>
       <c r="O24" s="2">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="P24" s="2">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="Q24" s="2">
         <v>-0.2</v>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>11.333333333333336</v>
+        <v>16.93333333333333</v>
       </c>
       <c r="W24" s="2">
         <v>12.8</v>
@@ -3188,10 +3188,10 @@
         <v>0.03</v>
       </c>
       <c r="O28">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="P28">
-        <v>-4</v>
+        <v>-8</v>
       </c>
       <c r="Q28">
         <v>0.05</v>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="U28" s="1">
         <f t="shared" si="1"/>
-        <v>4.2166666666666668</v>
+        <v>9.8166666666666664</v>
       </c>
       <c r="X28">
         <f t="shared" si="2"/>
@@ -3260,10 +3260,10 @@
         <v>0.24</v>
       </c>
       <c r="O29" s="2">
-        <v>-16</v>
+        <v>-20</v>
       </c>
       <c r="P29" s="2">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="Q29" s="2">
         <v>-0.15</v>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>11.25</v>
+        <v>16.850000000000001</v>
       </c>
       <c r="W29" s="2">
         <v>17.399999999999999</v>
@@ -3338,10 +3338,10 @@
         <v>0.05</v>
       </c>
       <c r="O30">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="P30">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="Q30">
         <v>0.1</v>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="U30" s="1">
         <f t="shared" si="1"/>
-        <v>11.700000000000001</v>
+        <v>17.3</v>
       </c>
       <c r="W30">
         <v>3.84</v>
@@ -3416,10 +3416,10 @@
         <v>0.25</v>
       </c>
       <c r="O31" s="2">
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="P31" s="2">
-        <v>-16</v>
+        <v>-20</v>
       </c>
       <c r="Q31" s="2">
         <v>-0.1</v>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="U31" s="1">
         <f t="shared" si="1"/>
-        <v>12.200000000000001</v>
+        <v>17.8</v>
       </c>
       <c r="W31" s="2">
         <v>16.760000000000002</v>
@@ -3494,10 +3494,10 @@
         <v>0.06</v>
       </c>
       <c r="O32">
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="P32">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="Q32">
         <v>0.1</v>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="U32" s="1">
         <f t="shared" si="1"/>
-        <v>12.1</v>
+        <v>17.7</v>
       </c>
       <c r="W32">
         <v>4.4000000000000004</v>
@@ -3569,10 +3569,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O33">
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="P33">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="Q33">
         <v>0.05</v>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="U33" s="1">
         <f t="shared" si="1"/>
-        <v>12.149999999999999</v>
+        <v>17.75</v>
       </c>
       <c r="W33">
         <v>4.8</v>
@@ -3647,10 +3647,10 @@
         <v>0.27</v>
       </c>
       <c r="O34" s="2">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="P34" s="2">
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="Q34" s="2">
         <v>-0.05</v>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="U34" s="1">
         <f t="shared" si="1"/>
-        <v>10.816666666666666</v>
+        <v>16.416666666666668</v>
       </c>
       <c r="X34" s="2">
         <f t="shared" si="2"/>
@@ -3719,10 +3719,10 @@
         <v>0.32</v>
       </c>
       <c r="O35" s="2">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="P35" s="2">
-        <v>-16</v>
+        <v>-20</v>
       </c>
       <c r="Q35" s="2">
         <v>-0.1</v>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="U35" s="1">
         <f t="shared" si="1"/>
-        <v>10.733333333333333</v>
+        <v>16.333333333333336</v>
       </c>
       <c r="W35" s="2">
         <v>22.2</v>
@@ -3770,10 +3770,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O36">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="P36">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="Q36">
         <v>0.1</v>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="U36" s="1">
         <f t="shared" si="1"/>
-        <v>12.100000000000001</v>
+        <v>17.7</v>
       </c>
       <c r="W36">
         <v>3.8</v>
@@ -3820,10 +3820,10 @@
         <v>0.05</v>
       </c>
       <c r="O37">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="P37">
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="Q37">
         <v>0.05</v>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="1"/>
-        <v>12.149999999999999</v>
+        <v>17.75</v>
       </c>
       <c r="W37">
         <v>3.6</v>
@@ -3870,10 +3870,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="O38" s="4">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="P38" s="4">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="Q38" s="4">
         <v>-0.05</v>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>12.716666666666665</v>
+        <v>18.316666666666663</v>
       </c>
       <c r="W38" s="4">
         <v>9.5</v>
@@ -4016,10 +4016,10 @@
         <v>0.05</v>
       </c>
       <c r="O41">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="P41">
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="Q41">
         <v>0</v>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="U41" s="1">
         <f t="shared" si="1"/>
-        <v>11.766666666666666</v>
+        <v>17.366666666666667</v>
       </c>
       <c r="X41">
         <f>W41*0.015</f>
@@ -4085,10 +4085,10 @@
         <v>0.06</v>
       </c>
       <c r="O42">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="P42">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="Q42">
         <v>0.05</v>
@@ -4104,7 +4104,7 @@
       </c>
       <c r="U42" s="1">
         <f t="shared" ref="U42:U44" si="4">M42-N42*20-O42*0.8-P42*0.6-Q42*5+R42*10+S42/300</f>
-        <v>11.549999999999999</v>
+        <v>17.150000000000002</v>
       </c>
       <c r="X42">
         <f>W42*0.015</f>
@@ -4157,10 +4157,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O43">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="P43">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="Q43">
         <v>0</v>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="U43" s="1">
         <f t="shared" si="4"/>
-        <v>11.8</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="X43">
         <f>W43*0.015</f>
@@ -4202,10 +4202,10 @@
         <v>0.22</v>
       </c>
       <c r="O44">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="P44">
-        <v>-15</v>
+        <v>-19</v>
       </c>
       <c r="Q44">
         <v>-0.1</v>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="U44" s="1">
         <f t="shared" si="4"/>
-        <v>12.116666666666667</v>
+        <v>17.716666666666669</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tweak 556 muzzles AGAIN
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89345487-2219-4402-8225-DB8C2CC9C189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F300C9-EE8A-4750-9BE5-CD31FE53112C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,7 +1499,7 @@
         <v>0.09</v>
       </c>
       <c r="O5" s="2">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="P5" s="2">
         <v>-13</v>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="U5" s="1">
         <f t="shared" si="1"/>
-        <v>17.816666666666666</v>
+        <v>17.016666666666669</v>
       </c>
       <c r="W5" s="2">
         <v>6</v>
@@ -1577,7 +1577,7 @@
         <v>0.12</v>
       </c>
       <c r="O6" s="2">
-        <v>-17</v>
+        <v>-16</v>
       </c>
       <c r="P6" s="2">
         <v>-14</v>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="U6" s="1">
         <f t="shared" si="1"/>
-        <v>17.933333333333337</v>
+        <v>17.133333333333336</v>
       </c>
       <c r="W6" s="2">
         <v>8</v>
@@ -1655,7 +1655,7 @@
         <v>0.15</v>
       </c>
       <c r="O7" s="2">
-        <v>-18</v>
+        <v>-17</v>
       </c>
       <c r="P7" s="2">
         <v>-15</v>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="U7" s="1">
         <f t="shared" si="1"/>
-        <v>17.7</v>
+        <v>16.900000000000002</v>
       </c>
       <c r="W7" s="2">
         <v>10</v>
@@ -1889,13 +1889,13 @@
         <v>0.12</v>
       </c>
       <c r="O10" s="4">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="P10" s="4">
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="Q10" s="4">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="R10" s="4">
         <v>0.02</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="U10" s="1">
         <f t="shared" si="1"/>
-        <v>17.783333333333335</v>
+        <v>17.133333333333329</v>
       </c>
       <c r="W10" s="4">
         <v>7.8</v>
@@ -1967,7 +1967,7 @@
         <v>0.25</v>
       </c>
       <c r="O11" s="2">
-        <v>-19</v>
+        <v>-18</v>
       </c>
       <c r="P11" s="2">
         <v>-17</v>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="U11" s="1">
         <f t="shared" si="1"/>
-        <v>18.366666666666664</v>
+        <v>17.566666666666666</v>
       </c>
       <c r="W11" s="2">
         <v>17</v>
@@ -2117,16 +2117,16 @@
         <v>-3.2499999999999991</v>
       </c>
       <c r="M13" s="2">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="N13" s="2">
         <v>0.3</v>
       </c>
       <c r="O13" s="2">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="P13" s="2">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="Q13" s="2">
         <v>-0.25</v>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="1"/>
-        <v>16.183333333333334</v>
+        <v>15.383333333333335</v>
       </c>
       <c r="W13" s="2">
         <v>22</v>
@@ -2357,7 +2357,7 @@
         <v>0.3</v>
       </c>
       <c r="O16" s="2">
-        <v>-17</v>
+        <v>-16</v>
       </c>
       <c r="P16" s="2">
         <v>-21</v>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="U16" s="1">
         <f t="shared" si="1"/>
-        <v>17.700000000000003</v>
+        <v>16.900000000000002</v>
       </c>
       <c r="W16" s="2">
         <v>22</v>
@@ -2513,7 +2513,7 @@
         <v>0.2</v>
       </c>
       <c r="O18" s="2">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="P18" s="2">
         <v>-16</v>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>17.899999999999999</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="W18" s="2">
         <v>13.9</v>
@@ -2591,7 +2591,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="O19" s="2">
-        <v>-19</v>
+        <v>-18</v>
       </c>
       <c r="P19" s="2">
         <v>-19</v>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="U19" s="1">
         <f t="shared" si="1"/>
-        <v>18.05</v>
+        <v>17.25</v>
       </c>
       <c r="W19" s="2">
         <v>19.2</v>
@@ -2885,7 +2885,7 @@
         <v>0.19</v>
       </c>
       <c r="O24" s="2">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="P24" s="2">
         <v>-17</v>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="U24" s="1">
         <f t="shared" si="1"/>
-        <v>16.93333333333333</v>
+        <v>16.133333333333333</v>
       </c>
       <c r="W24" s="2">
         <v>12.8</v>
@@ -3260,7 +3260,7 @@
         <v>0.24</v>
       </c>
       <c r="O29" s="2">
-        <v>-20</v>
+        <v>-19</v>
       </c>
       <c r="P29" s="2">
         <v>-14</v>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="U29" s="1">
         <f t="shared" si="1"/>
-        <v>16.850000000000001</v>
+        <v>16.05</v>
       </c>
       <c r="W29" s="2">
         <v>17.399999999999999</v>
@@ -3416,7 +3416,7 @@
         <v>0.25</v>
       </c>
       <c r="O31" s="2">
-        <v>-18</v>
+        <v>-17</v>
       </c>
       <c r="P31" s="2">
         <v>-20</v>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="U31" s="1">
         <f t="shared" si="1"/>
-        <v>17.8</v>
+        <v>17.000000000000004</v>
       </c>
       <c r="W31" s="2">
         <v>16.760000000000002</v>
@@ -3647,7 +3647,7 @@
         <v>0.27</v>
       </c>
       <c r="O34" s="2">
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="P34" s="2">
         <v>-19</v>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="U34" s="1">
         <f t="shared" si="1"/>
-        <v>16.416666666666668</v>
+        <v>15.616666666666667</v>
       </c>
       <c r="X34" s="2">
         <f t="shared" si="2"/>
@@ -3719,7 +3719,7 @@
         <v>0.32</v>
       </c>
       <c r="O35" s="2">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="P35" s="2">
         <v>-20</v>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="U35" s="1">
         <f t="shared" si="1"/>
-        <v>16.333333333333336</v>
+        <v>15.533333333333331</v>
       </c>
       <c r="W35" s="2">
         <v>22.2</v>
@@ -3873,10 +3873,10 @@
         <v>-13</v>
       </c>
       <c r="P38" s="4">
-        <v>-17</v>
+        <v>-15</v>
       </c>
       <c r="Q38" s="4">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="R38" s="4">
         <v>0.02</v>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="U38" s="1">
         <f t="shared" si="1"/>
-        <v>18.316666666666663</v>
+        <v>16.866666666666667</v>
       </c>
       <c r="W38" s="4">
         <v>9.5</v>

</xml_diff>

<commit_message>
add car15 flash moderator
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F300C9-EE8A-4750-9BE5-CD31FE53112C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904B34E9-0559-4180-AFFF-2E29EA725FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
   <si>
     <t>OLD</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>Steyr Breezer UMS 5.56x45 AUG Suppressor</t>
+  </si>
+  <si>
+    <t>colt_607_car15_3.5inch_flash_moderator</t>
+  </si>
+  <si>
+    <t>Colt 607 CAR-15 3.5" Flash Moderator</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z45"/>
+  <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1339,7 @@
         <v>750</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K35" si="0">C3-D3*20-E3*0.8-F3*0.6-G3*5+H3*5+I3/300</f>
+        <f t="shared" ref="K3:K36" si="0">C3-D3*20-E3*0.8-F3*0.6-G3*5+H3*5+I3/300</f>
         <v>3.0833333333333339</v>
       </c>
       <c r="M3">
@@ -1361,7 +1367,7 @@
         <v>500</v>
       </c>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:U41" si="1">M3-N3*20-O3*0.8-P3*0.6-Q3*5+R3*10+S3/300</f>
+        <f t="shared" ref="U3:U42" si="1">M3-N3*20-O3*0.8-P3*0.6-Q3*5+R3*10+S3/300</f>
         <v>17.350000000000001</v>
       </c>
       <c r="W3">
@@ -1446,14 +1452,14 @@
         <v>3.8</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X38" si="2">W4*0.015</f>
+        <f t="shared" ref="X4:X39" si="2">W4*0.015</f>
         <v>5.6999999999999995E-2</v>
       </c>
       <c r="Y4">
         <v>137</v>
       </c>
       <c r="Z4">
-        <f t="shared" ref="Z4:Z37" si="3">Y4+400</f>
+        <f t="shared" ref="Z4:Z38" si="3">Y4+400</f>
         <v>537</v>
       </c>
     </row>
@@ -2843,1146 +2849,1118 @@
         <v>408.99</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>0.09</v>
+      </c>
+      <c r="O24">
+        <v>-11</v>
+      </c>
+      <c r="P24">
+        <v>-12</v>
+      </c>
+      <c r="Q24">
+        <v>0.1</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>500</v>
+      </c>
+      <c r="U24" s="1">
+        <f t="shared" si="1"/>
+        <v>15.7</v>
+      </c>
+      <c r="W24">
+        <v>6.5</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="2"/>
+        <v>9.7500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>-7</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>-6</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <v>-7</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G25" s="2">
         <v>-0.3</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H25" s="2">
         <v>0.15</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I25" s="2">
         <v>140</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J25" s="2">
         <v>2000</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K25" s="3">
         <f t="shared" si="0"/>
         <v>-0.88333333333333386</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M25" s="2">
         <v>-5</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N25" s="2">
         <v>0.19</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O25" s="2">
         <v>-15</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P25" s="2">
         <v>-17</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="Q25" s="2">
         <v>-0.2</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R25" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S25" s="2">
         <v>100</v>
       </c>
-      <c r="T24" s="2">
+      <c r="T25" s="2">
         <v>1300</v>
       </c>
-      <c r="U24" s="1">
+      <c r="U25" s="1">
         <f t="shared" si="1"/>
         <v>16.133333333333333</v>
       </c>
-      <c r="W24" s="2">
+      <c r="W25" s="2">
         <v>12.8</v>
       </c>
-      <c r="X24" s="2">
+      <c r="X25" s="2">
         <f t="shared" si="2"/>
         <v>0.192</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="Y25" s="2">
         <v>999</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="Z25" s="2">
         <f t="shared" si="3"/>
         <v>1399</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>-2</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>0.12</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>-2</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>-2</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>0.15</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>0.05</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <v>80</v>
       </c>
-      <c r="J25">
+      <c r="J26">
         <v>1000</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K26" s="1">
         <f t="shared" si="0"/>
         <v>-1.8333333333333339</v>
       </c>
-      <c r="M25">
+      <c r="M26">
         <v>-2</v>
       </c>
-      <c r="N25">
+      <c r="N26">
         <v>0.16</v>
       </c>
-      <c r="O25">
+      <c r="O26">
         <v>-2</v>
       </c>
-      <c r="P25">
+      <c r="P26">
         <v>-2</v>
       </c>
-      <c r="Q25">
+      <c r="Q26">
         <v>0.24</v>
       </c>
-      <c r="R25">
+      <c r="R26">
         <v>0.08</v>
       </c>
-      <c r="S25">
+      <c r="S26">
         <v>80</v>
       </c>
-      <c r="T25">
+      <c r="T26">
         <v>600</v>
       </c>
-      <c r="U25" s="1">
+      <c r="U26" s="1">
         <f t="shared" si="1"/>
         <v>-2.5333333333333341</v>
       </c>
-      <c r="X25">
+      <c r="X26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y25">
+      <c r="Y26">
         <v>59.99</v>
       </c>
-      <c r="Z25">
+      <c r="Z26">
         <f t="shared" si="3"/>
         <v>459.99</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>63</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>-1.5</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>0.09</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>-1</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>-1</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>0.1</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <v>60</v>
       </c>
-      <c r="J26">
+      <c r="J27">
         <v>750</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K27" s="1">
         <f t="shared" si="0"/>
         <v>-2.1999999999999997</v>
       </c>
-      <c r="M26">
+      <c r="M27">
         <v>-1</v>
       </c>
-      <c r="N26">
+      <c r="N27">
         <v>0.08</v>
       </c>
-      <c r="O26">
+      <c r="O27">
         <v>-1</v>
       </c>
-      <c r="P26">
+      <c r="P27">
         <v>-1</v>
       </c>
-      <c r="Q26">
+      <c r="Q27">
         <v>0.12</v>
       </c>
-      <c r="R26">
+      <c r="R27">
         <v>0.04</v>
       </c>
-      <c r="S26">
+      <c r="S27">
         <v>40</v>
       </c>
-      <c r="T26">
+      <c r="T27">
         <v>500</v>
       </c>
-      <c r="U26" s="1">
+      <c r="U27" s="1">
         <f t="shared" si="1"/>
         <v>-1.2666666666666671</v>
       </c>
-      <c r="X26">
+      <c r="X27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y26">
+      <c r="Y27">
         <v>44.99</v>
       </c>
-      <c r="Z26">
+      <c r="Z27">
         <f t="shared" si="3"/>
         <v>444.99</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>65</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>66</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>-1</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>0.06</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>0.05</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <v>40</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <v>500</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K28" s="1">
         <f t="shared" si="0"/>
         <v>-2.3166666666666669</v>
       </c>
-      <c r="M27">
+      <c r="M28">
         <v>-0.5</v>
       </c>
-      <c r="N27">
+      <c r="N28">
         <v>0.04</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
         <v>0.06</v>
       </c>
-      <c r="R27">
+      <c r="R28">
         <v>0.02</v>
       </c>
-      <c r="S27">
+      <c r="S28">
         <v>20</v>
       </c>
-      <c r="T27">
+      <c r="T28">
         <v>400</v>
       </c>
-      <c r="U27" s="1">
+      <c r="U28" s="1">
         <f t="shared" si="1"/>
         <v>-1.3333333333333335</v>
       </c>
-      <c r="X27">
+      <c r="X28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y27">
+      <c r="Y28">
         <v>29.99</v>
       </c>
-      <c r="Z27">
+      <c r="Z28">
         <f t="shared" si="3"/>
         <v>429.99</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>68</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>-1</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>0.03</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <v>2</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>0.1</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>5</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>300</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K29" s="1">
         <f t="shared" si="0"/>
         <v>-3.2833333333333332</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <v>0.03</v>
       </c>
-      <c r="O28">
+      <c r="O29">
         <v>-7</v>
       </c>
-      <c r="P28">
+      <c r="P29">
         <v>-8</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>0.05</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>0.02</v>
       </c>
-      <c r="S28">
+      <c r="S29">
         <v>20</v>
       </c>
-      <c r="T28">
+      <c r="T29">
         <v>300</v>
       </c>
-      <c r="U28" s="1">
+      <c r="U29" s="1">
         <f t="shared" si="1"/>
         <v>9.8166666666666664</v>
       </c>
-      <c r="X28">
+      <c r="X29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z28">
+      <c r="Z29">
         <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C30" s="2">
         <v>-16</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D30" s="2">
         <v>0.3</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E30" s="2">
         <v>-6</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F30" s="2">
         <v>-12</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G30" s="2">
         <v>-0.3</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H30" s="2">
         <v>0.1</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I30" s="2">
         <v>200</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J30" s="2">
         <v>1500</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K30" s="3">
         <f t="shared" si="0"/>
         <v>-7.333333333333333</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M30" s="2">
         <v>-5</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N30" s="2">
         <v>0.24</v>
       </c>
-      <c r="O29" s="2">
+      <c r="O30" s="2">
         <v>-19</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P30" s="2">
         <v>-14</v>
       </c>
-      <c r="Q29" s="2">
+      <c r="Q30" s="2">
         <v>-0.15</v>
       </c>
-      <c r="R29" s="2">
+      <c r="R30" s="2">
         <v>0.12</v>
       </c>
-      <c r="S29" s="2">
+      <c r="S30" s="2">
         <v>90</v>
       </c>
-      <c r="T29" s="2">
+      <c r="T30" s="2">
         <v>1400</v>
       </c>
-      <c r="U29" s="1">
+      <c r="U30" s="1">
         <f t="shared" si="1"/>
         <v>16.05</v>
       </c>
-      <c r="W29" s="2">
+      <c r="W30" s="2">
         <v>17.399999999999999</v>
       </c>
-      <c r="X29" s="2">
+      <c r="X30" s="2">
         <f t="shared" si="2"/>
         <v>0.26099999999999995</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="Y30" s="2">
         <v>1099</v>
       </c>
-      <c r="Z29" s="2">
+      <c r="Z30" s="2">
         <f t="shared" si="3"/>
         <v>1499</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>72</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>-1</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>0.04</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>-3</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>-1</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>0.1</v>
       </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <v>5</v>
       </c>
-      <c r="J30">
+      <c r="J31">
         <v>300</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K31" s="1">
         <f t="shared" si="0"/>
         <v>0.7166666666666669</v>
       </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
         <v>0.05</v>
       </c>
-      <c r="O30">
+      <c r="O31">
         <v>-16</v>
       </c>
-      <c r="P30">
+      <c r="P31">
         <v>-10</v>
       </c>
-      <c r="Q30">
+      <c r="Q31">
         <v>0.1</v>
       </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-      <c r="T30">
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
         <v>500</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U31" s="1">
         <f t="shared" si="1"/>
         <v>17.3</v>
       </c>
-      <c r="W30">
+      <c r="W31">
         <v>3.84</v>
       </c>
-      <c r="X30">
+      <c r="X31">
         <f t="shared" si="2"/>
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="Y30">
+      <c r="Y31">
         <v>151</v>
       </c>
-      <c r="Z30">
+      <c r="Z31">
         <f t="shared" si="3"/>
         <v>551</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <v>-11</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <v>0.24</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E32" s="2">
         <v>-3</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F32" s="2">
         <v>-9</v>
       </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
         <v>0.2</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I32" s="2">
         <v>100</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J32" s="2">
         <v>1300</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K32" s="3">
         <f t="shared" si="0"/>
         <v>-6.666666666666667</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M32" s="2">
         <v>-6</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N32" s="2">
         <v>0.25</v>
       </c>
-      <c r="O31" s="2">
+      <c r="O32" s="2">
         <v>-17</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P32" s="2">
         <v>-20</v>
       </c>
-      <c r="Q31" s="2">
+      <c r="Q32" s="2">
         <v>-0.1</v>
       </c>
-      <c r="R31" s="2">
+      <c r="R32" s="2">
         <v>0.16</v>
       </c>
-      <c r="S31" s="2">
+      <c r="S32" s="2">
         <v>90</v>
       </c>
-      <c r="T31" s="2">
+      <c r="T32" s="2">
         <v>1200</v>
       </c>
-      <c r="U31" s="1">
+      <c r="U32" s="1">
         <f t="shared" si="1"/>
         <v>17.000000000000004</v>
       </c>
-      <c r="W31" s="2">
+      <c r="W32" s="2">
         <v>16.760000000000002</v>
       </c>
-      <c r="X31" s="2">
+      <c r="X32" s="2">
         <f t="shared" si="2"/>
         <v>0.25140000000000001</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="Y32" s="2">
         <v>899.99</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="Z32" s="2">
         <f t="shared" si="3"/>
         <v>1299.99</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>75</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>76</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>-2</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>0.05</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>-5</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>-6</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>0.2</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
         <v>50</v>
       </c>
-      <c r="J32">
+      <c r="J33">
         <v>750</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K33" s="1">
         <f t="shared" si="0"/>
         <v>3.7666666666666662</v>
       </c>
-      <c r="M32">
+      <c r="M33">
         <v>-1</v>
       </c>
-      <c r="N32">
+      <c r="N33">
         <v>0.06</v>
       </c>
-      <c r="O32">
+      <c r="O33">
         <v>-18</v>
       </c>
-      <c r="P32">
+      <c r="P33">
         <v>-10</v>
       </c>
-      <c r="Q32">
+      <c r="Q33">
         <v>0.1</v>
       </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-      <c r="T32">
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
         <v>400</v>
       </c>
-      <c r="U32" s="1">
+      <c r="U33" s="1">
         <f t="shared" si="1"/>
         <v>17.7</v>
       </c>
-      <c r="W32">
+      <c r="W33">
         <v>4.4000000000000004</v>
       </c>
-      <c r="X32">
+      <c r="X33">
         <f t="shared" si="2"/>
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="Z32">
+      <c r="Z33">
         <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>77</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>78</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>-0.5</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>-5</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>-5</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>0.05</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <v>0.05</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>30</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>1000</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K34" s="1">
         <f t="shared" si="0"/>
         <v>5.1999999999999993</v>
       </c>
-      <c r="M33">
+      <c r="M34">
         <v>1</v>
       </c>
-      <c r="N33">
+      <c r="N34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O33">
+      <c r="O34">
         <v>-11</v>
       </c>
-      <c r="P33">
+      <c r="P34">
         <v>-16</v>
       </c>
-      <c r="Q33">
+      <c r="Q34">
         <v>0.05</v>
       </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-      <c r="T33">
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
         <v>500</v>
       </c>
-      <c r="U33" s="1">
+      <c r="U34" s="1">
         <f t="shared" si="1"/>
         <v>17.75</v>
       </c>
-      <c r="W33">
+      <c r="W34">
         <v>4.8</v>
       </c>
-      <c r="X33">
+      <c r="X34">
         <f t="shared" si="2"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="Y33">
+      <c r="Y34">
         <v>64.989999999999995</v>
       </c>
-      <c r="Z33">
+      <c r="Z34">
         <f t="shared" si="3"/>
         <v>464.99</v>
       </c>
     </row>
-    <row r="34" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C35" s="2">
         <v>-6.5</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D35" s="2">
         <v>0.27</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E35" s="2">
         <v>-6</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F35" s="2">
         <v>-10</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G35" s="2">
         <v>-0.5</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H35" s="2">
         <v>0.1</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I35" s="2">
         <v>250</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J35" s="2">
         <v>2000</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K35" s="3">
         <f t="shared" si="0"/>
         <v>2.7333333333333338</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M35" s="2">
         <v>-2</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N35" s="2">
         <v>0.27</v>
       </c>
-      <c r="O34" s="2">
+      <c r="O35" s="2">
         <v>-13</v>
       </c>
-      <c r="P34" s="2">
+      <c r="P35" s="2">
         <v>-19</v>
       </c>
-      <c r="Q34" s="2">
+      <c r="Q35" s="2">
         <v>-0.05</v>
       </c>
-      <c r="R34" s="2">
+      <c r="R35" s="2">
         <v>0.08</v>
       </c>
-      <c r="S34" s="2">
+      <c r="S35" s="2">
         <v>50</v>
       </c>
-      <c r="T34" s="2">
+      <c r="T35" s="2">
         <v>1500</v>
       </c>
-      <c r="U34" s="1">
+      <c r="U35" s="1">
         <f t="shared" si="1"/>
         <v>15.616666666666667</v>
       </c>
-      <c r="X34" s="2">
+      <c r="X35" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="Z35" s="2">
         <f t="shared" si="3"/>
         <v>400</v>
       </c>
     </row>
-    <row r="35" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C36" s="2">
         <v>-8</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D36" s="2">
         <v>0.32</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E36" s="2">
         <v>-6</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F36" s="2">
         <v>-12</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G36" s="2">
         <v>-0.5</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H36" s="2">
         <v>0.2</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I36" s="2">
         <v>400</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J36" s="2">
         <v>2000</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K36" s="3">
         <f t="shared" si="0"/>
         <v>2.4333333333333327</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M36" s="2">
         <v>-4</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N36" s="2">
         <v>0.32</v>
       </c>
-      <c r="O35" s="2">
+      <c r="O36" s="2">
         <v>-15</v>
       </c>
-      <c r="P35" s="2">
+      <c r="P36" s="2">
         <v>-20</v>
       </c>
-      <c r="Q35" s="2">
+      <c r="Q36" s="2">
         <v>-0.1</v>
       </c>
-      <c r="R35" s="2">
+      <c r="R36" s="2">
         <v>0.12</v>
       </c>
-      <c r="S35" s="2">
+      <c r="S36" s="2">
         <v>70</v>
       </c>
-      <c r="T35" s="2">
+      <c r="T36" s="2">
         <v>1600</v>
       </c>
-      <c r="U35" s="1">
+      <c r="U36" s="1">
         <f t="shared" si="1"/>
         <v>15.533333333333331</v>
       </c>
-      <c r="W35" s="2">
+      <c r="W36" s="2">
         <v>22.2</v>
       </c>
-      <c r="X35" s="2">
+      <c r="X36" s="2">
         <f t="shared" si="2"/>
         <v>0.33299999999999996</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="Y36" s="2">
         <v>797.99</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="Z36" s="2">
         <f t="shared" si="3"/>
         <v>1197.99</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>93</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>94</v>
       </c>
-      <c r="K36" s="1"/>
-      <c r="M36">
+      <c r="K37" s="1"/>
+      <c r="M37">
         <v>-1</v>
       </c>
-      <c r="N36">
+      <c r="N37">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O36">
+      <c r="O37">
         <v>-16</v>
       </c>
-      <c r="P36">
+      <c r="P37">
         <v>-13</v>
       </c>
-      <c r="Q36">
+      <c r="Q37">
         <v>0.1</v>
       </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
-      <c r="T36">
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
         <v>600</v>
       </c>
-      <c r="U36" s="1">
+      <c r="U37" s="1">
         <f t="shared" si="1"/>
         <v>17.7</v>
       </c>
-      <c r="W36">
+      <c r="W37">
         <v>3.8</v>
       </c>
-      <c r="X36">
+      <c r="X37">
         <f t="shared" si="2"/>
         <v>5.6999999999999995E-2</v>
       </c>
-      <c r="Y36">
+      <c r="Y37">
         <v>200</v>
       </c>
-      <c r="Z36">
+      <c r="Z37">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>99</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>101</v>
       </c>
-      <c r="M37">
+      <c r="M38">
         <v>-1</v>
       </c>
-      <c r="N37">
+      <c r="N38">
         <v>0.05</v>
       </c>
-      <c r="O37">
+      <c r="O38">
         <v>-13</v>
       </c>
-      <c r="P37">
+      <c r="P38">
         <v>-16</v>
       </c>
-      <c r="Q37">
+      <c r="Q38">
         <v>0.05</v>
       </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
         <v>500</v>
       </c>
-      <c r="U37" s="1">
+      <c r="U38" s="1">
         <f t="shared" si="1"/>
         <v>17.75</v>
       </c>
-      <c r="W37">
+      <c r="W38">
         <v>3.6</v>
       </c>
-      <c r="X37">
+      <c r="X38">
         <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="Y37">
+      <c r="Y38">
         <v>43.95</v>
       </c>
-      <c r="Z37">
+      <c r="Z38">
         <f t="shared" si="3"/>
         <v>443.95</v>
       </c>
     </row>
-    <row r="38" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
+      <c r="M39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="O38" s="4">
+      <c r="O39" s="4">
         <v>-13</v>
       </c>
-      <c r="P38" s="4">
+      <c r="P39" s="4">
         <v>-15</v>
       </c>
-      <c r="Q38" s="4">
-        <v>0</v>
-      </c>
-      <c r="R38" s="4">
+      <c r="Q39" s="4">
+        <v>0</v>
+      </c>
+      <c r="R39" s="4">
         <v>0.02</v>
       </c>
-      <c r="S38" s="4">
+      <c r="S39" s="4">
         <v>20</v>
       </c>
-      <c r="T38" s="4">
+      <c r="T39" s="4">
         <v>1000</v>
       </c>
-      <c r="U38" s="1">
+      <c r="U39" s="1">
         <f t="shared" si="1"/>
         <v>16.866666666666667</v>
       </c>
-      <c r="W38" s="4">
+      <c r="W39" s="4">
         <v>9.5</v>
       </c>
-      <c r="X38" s="4">
+      <c r="X39" s="4">
         <f t="shared" si="2"/>
         <v>0.14249999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U39" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40">
-        <v>-2</v>
-      </c>
-      <c r="D40">
-        <v>0.05</v>
-      </c>
-      <c r="E40">
-        <v>5</v>
-      </c>
-      <c r="F40">
-        <v>5</v>
-      </c>
-      <c r="G40">
-        <v>0.1</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>-50</v>
-      </c>
-      <c r="J40">
-        <v>1500</v>
-      </c>
-      <c r="K40" s="1">
-        <f>C40-D40*20-E40*0.8-F40*0.6-G40*5+H40*5+I40/300</f>
-        <v>-10.666666666666666</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0.04</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0.1</v>
-      </c>
-      <c r="R40">
-        <v>0.02</v>
-      </c>
-      <c r="S40">
-        <v>30</v>
-      </c>
-      <c r="T40">
-        <v>1500</v>
-      </c>
       <c r="U40" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="X40">
-        <f>W40*0.015</f>
-        <v>0</v>
-      </c>
-      <c r="Z40">
-        <f>Y40+400</f>
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C41">
         <v>-2</v>
@@ -3991,48 +3969,54 @@
         <v>0.05</v>
       </c>
       <c r="E41">
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H41">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>50</v>
+        <v>-50</v>
+      </c>
+      <c r="J41">
+        <v>1500</v>
       </c>
       <c r="K41" s="1">
         <f>C41-D41*20-E41*0.8-F41*0.6-G41*5+H41*5+I41/300</f>
-        <v>5.2166666666666677</v>
+        <v>-10.666666666666666</v>
       </c>
       <c r="M41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="O41">
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="P41">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R41">
         <v>0.02</v>
       </c>
       <c r="S41">
-        <v>50</v>
+        <v>30</v>
+      </c>
+      <c r="T41">
+        <v>1500</v>
       </c>
       <c r="U41" s="1">
         <f t="shared" si="1"/>
-        <v>17.366666666666667</v>
+        <v>-1</v>
       </c>
       <c r="X41">
         <f>W41*0.015</f>
@@ -4045,66 +4029,60 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42">
         <v>-2</v>
       </c>
       <c r="D42">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E42">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="F42">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
         <v>0.05</v>
       </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
       <c r="I42">
-        <v>120</v>
-      </c>
-      <c r="J42">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="K42" s="1">
         <f>C42-D42*20-E42*0.8-F42*0.6-G42*5+H42*5+I42/300</f>
-        <v>5.15</v>
+        <v>5.2166666666666677</v>
       </c>
       <c r="M42">
         <v>1</v>
       </c>
       <c r="N42">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="O42">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="P42">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="Q42">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="R42">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="S42">
-        <v>60</v>
-      </c>
-      <c r="T42">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" ref="U42:U44" si="4">M42-N42*20-O42*0.8-P42*0.6-Q42*5+R42*10+S42/300</f>
-        <v>17.150000000000002</v>
+        <f t="shared" si="1"/>
+        <v>17.366666666666667</v>
       </c>
       <c r="X42">
         <f>W42*0.015</f>
@@ -4117,66 +4095,66 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D43">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E43">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="F43">
-        <v>-7</v>
+        <v>-3</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J43">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="K43" s="1">
         <f>C43-D43*20-E43*0.8-F43*0.6-G43*5+H43*5+I43/300</f>
-        <v>5.8</v>
+        <v>5.15</v>
       </c>
       <c r="M43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N43">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="O43">
+        <v>-12</v>
+      </c>
+      <c r="P43">
         <v>-13</v>
       </c>
-      <c r="P43">
-        <v>-14</v>
-      </c>
       <c r="Q43">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R43">
         <v>0</v>
       </c>
       <c r="S43">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="T43">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="4"/>
-        <v>17.399999999999999</v>
+        <f t="shared" ref="U43:U45" si="4">M43-N43*20-O43*0.8-P43*0.6-Q43*5+R43*10+S43/300</f>
+        <v>17.150000000000002</v>
       </c>
       <c r="X43">
         <f>W43*0.015</f>
@@ -4189,43 +4167,115 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
-      </c>
-      <c r="K44" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="C44">
+        <v>-1</v>
+      </c>
+      <c r="D44">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E44">
+        <v>-5</v>
+      </c>
+      <c r="F44">
+        <v>-7</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>750</v>
+      </c>
+      <c r="K44" s="1">
+        <f>C44-D44*20-E44*0.8-F44*0.6-G44*5+H44*5+I44/300</f>
+        <v>5.8</v>
+      </c>
       <c r="M44">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="N44">
-        <v>0.22</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O44">
+        <v>-13</v>
+      </c>
+      <c r="P44">
         <v>-14</v>
       </c>
-      <c r="P44">
-        <v>-19</v>
-      </c>
       <c r="Q44">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="R44">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="S44">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="T44">
-        <v>1800</v>
+        <v>750</v>
       </c>
       <c r="U44" s="1">
         <f t="shared" si="4"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="X44">
+        <f>W44*0.015</f>
+        <v>0</v>
+      </c>
+      <c r="Z44">
+        <f>Y44+400</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="K45" s="1"/>
+      <c r="M45">
+        <v>-2</v>
+      </c>
+      <c r="N45">
+        <v>0.22</v>
+      </c>
+      <c r="O45">
+        <v>-14</v>
+      </c>
+      <c r="P45">
+        <v>-19</v>
+      </c>
+      <c r="Q45">
+        <v>-0.1</v>
+      </c>
+      <c r="R45">
+        <v>0.08</v>
+      </c>
+      <c r="S45">
+        <v>65</v>
+      </c>
+      <c r="T45">
+        <v>1800</v>
+      </c>
+      <c r="U45" s="1">
+        <f t="shared" si="4"/>
         <v>17.716666666666669</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U45" s="1"/>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 556 barrel extensions
</commit_message>
<xml_diff>
--- a/changes/556-muzzles.xlsx
+++ b/changes/556-muzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE5193E5-7644-4C17-9D44-F8A02A2334B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF36B18-ABD1-4CEB-9A66-F9080C1C01A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="5100" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="3615" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="556-muzzles" sheetId="1" r:id="rId1"/>
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3007,22 +3007,22 @@
         <v>-1.7083333333333339</v>
       </c>
       <c r="M26">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="N26">
         <v>0.16</v>
       </c>
       <c r="O26">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="P26">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Q26">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="R26">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="S26">
         <v>80</v>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="U26" s="1">
         <f t="shared" si="1"/>
-        <v>-2.7333333333333334</v>
+        <v>-5.4333333333333345</v>
       </c>
       <c r="X26">
         <f t="shared" si="2"/>
@@ -3082,22 +3082,22 @@
         <v>-2.4499999999999997</v>
       </c>
       <c r="M27">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N27">
         <v>0.08</v>
       </c>
       <c r="O27">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P27">
         <v>-1</v>
       </c>
       <c r="Q27">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="R27">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="S27">
         <v>40</v>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="U27" s="1">
         <f t="shared" si="1"/>
-        <v>-1.3666666666666667</v>
+        <v>-3.3166666666666669</v>
       </c>
       <c r="X27">
         <f t="shared" si="2"/>
@@ -3157,7 +3157,7 @@
         <v>-2.4416666666666669</v>
       </c>
       <c r="M28">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="N28">
         <v>0.04</v>
@@ -3169,10 +3169,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="R28">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="S28">
         <v>20</v>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="U28" s="1">
         <f t="shared" si="1"/>
-        <v>-1.3833333333333333</v>
+        <v>-1.9583333333333333</v>
       </c>
       <c r="X28">
         <f t="shared" si="2"/>

</xml_diff>